<commit_message>
Added TBB repository, Modified Comparison results
</commit_message>
<xml_diff>
--- a/docs/Comparison.xlsx
+++ b/docs/Comparison.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6510" yWindow="0" windowWidth="22110" windowHeight="9402"/>
+    <workbookView xWindow="7452" yWindow="0" windowWidth="22110" windowHeight="9402" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Graphs" sheetId="4" r:id="rId1"/>
@@ -106,9 +106,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -245,7 +244,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -264,13 +262,14 @@
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -11973,7 +11972,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="A72" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C102" sqref="C102"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData/>
@@ -11986,12 +11987,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:W116"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="8.578125" customWidth="1"/>
-    <col min="2" max="2" width="18.05078125" customWidth="1"/>
+    <col min="2" max="2" width="14.578125" customWidth="1"/>
     <col min="3" max="10" width="8.578125" style="9" customWidth="1"/>
     <col min="11" max="14" width="8.578125" customWidth="1"/>
   </cols>
@@ -12013,10 +12016,10 @@
       <c r="B5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="38" t="s">
+      <c r="C5" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="38"/>
+      <c r="D5" s="36"/>
     </row>
     <row r="6" spans="2:23" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" s="13" t="s">
@@ -12526,17 +12529,17 @@
       <c r="B22" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="38" t="s">
+      <c r="C22" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="D22" s="38"/>
+      <c r="D22" s="36"/>
       <c r="E22"/>
       <c r="F22"/>
       <c r="G22"/>
-      <c r="H22" s="39" t="s">
+      <c r="H22" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="I22" s="39"/>
+      <c r="I22" s="37"/>
       <c r="J22" s="5">
         <f>'Execution Time Records'!D20</f>
         <v>12455</v>
@@ -13446,9 +13449,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J35"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="2" max="2" width="14.578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="25.8" x14ac:dyDescent="0.95">
       <c r="B2" s="8" t="s">
@@ -13492,10 +13500,10 @@
       <c r="B5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="38" t="s">
+      <c r="C5" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="38"/>
+      <c r="D5" s="36"/>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
@@ -14014,14 +14022,14 @@
       <c r="B22" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="38" t="s">
+      <c r="C22" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="D22" s="38"/>
-      <c r="H22" s="39" t="s">
+      <c r="D22" s="36"/>
+      <c r="H22" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="I22" s="39"/>
+      <c r="I22" s="37"/>
       <c r="J22" s="5">
         <f>'Execution Time Records'!N20</f>
         <v>5993.2</v>
@@ -14525,7 +14533,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:T116"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -14580,55 +14590,55 @@
       <c r="B3" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="30">
+      <c r="C3" s="29">
         <v>1</v>
       </c>
-      <c r="D3" s="30">
+      <c r="D3" s="29">
         <v>2</v>
       </c>
-      <c r="E3" s="30">
+      <c r="E3" s="29">
         <v>3</v>
       </c>
-      <c r="F3" s="30">
+      <c r="F3" s="29">
         <v>4</v>
       </c>
-      <c r="G3" s="30">
+      <c r="G3" s="29">
         <v>5</v>
       </c>
-      <c r="H3" s="30">
+      <c r="H3" s="29">
         <v>6</v>
       </c>
-      <c r="I3" s="30">
+      <c r="I3" s="29">
         <v>7</v>
       </c>
-      <c r="J3" s="30">
+      <c r="J3" s="29">
         <v>8</v>
       </c>
-      <c r="L3" s="29" t="s">
+      <c r="L3" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="30">
+      <c r="M3" s="29">
         <v>1</v>
       </c>
-      <c r="N3" s="30">
+      <c r="N3" s="29">
         <v>2</v>
       </c>
-      <c r="O3" s="30">
+      <c r="O3" s="29">
         <v>3</v>
       </c>
-      <c r="P3" s="30">
+      <c r="P3" s="29">
         <v>4</v>
       </c>
-      <c r="Q3" s="30">
+      <c r="Q3" s="29">
         <v>5</v>
       </c>
-      <c r="R3" s="30">
+      <c r="R3" s="29">
         <v>6</v>
       </c>
-      <c r="S3" s="30">
+      <c r="S3" s="29">
         <v>7</v>
       </c>
-      <c r="T3" s="30">
+      <c r="T3" s="29">
         <v>8</v>
       </c>
     </row>
@@ -14636,70 +14646,70 @@
       <c r="B4" s="15">
         <v>1</v>
       </c>
-      <c r="C4" s="28">
+      <c r="C4" s="38">
         <f t="shared" ref="C4:C15" si="0">$D21/$N21</f>
         <v>2.1350202563591685</v>
       </c>
-      <c r="D4" s="28">
+      <c r="D4" s="38">
         <f t="shared" ref="D4:D15" si="1">$D33/$N33</f>
         <v>2.1567013003986149</v>
       </c>
-      <c r="E4" s="28">
+      <c r="E4" s="38">
         <f t="shared" ref="E4:E15" si="2">$D45/$N45</f>
         <v>2.199879550321199</v>
       </c>
-      <c r="F4" s="28">
+      <c r="F4" s="38">
         <f t="shared" ref="F4:F15" si="3">$D57/$N57</f>
         <v>2.1437529029261495</v>
       </c>
-      <c r="G4" s="28">
+      <c r="G4" s="38">
         <f t="shared" ref="G4:G15" si="4">$D69/$N69</f>
         <v>2.1038999506335361</v>
       </c>
-      <c r="H4" s="28">
+      <c r="H4" s="38">
         <f t="shared" ref="H4:H15" si="5">$D81/$N81</f>
         <v>2.1126585182029687</v>
       </c>
-      <c r="I4" s="28">
+      <c r="I4" s="38">
         <f t="shared" ref="I4:I15" si="6">$D93/$N93</f>
         <v>2.1642545598731164</v>
       </c>
-      <c r="J4" s="28">
+      <c r="J4" s="38">
         <f t="shared" ref="J4:J15" si="7">$D105/$N105</f>
         <v>2.1412559749464317</v>
       </c>
-      <c r="L4" s="31">
+      <c r="L4" s="30">
         <v>1</v>
       </c>
-      <c r="M4" s="28">
+      <c r="M4" s="38">
         <f>$N21/$D21</f>
         <v>0.46837963106977326</v>
       </c>
-      <c r="N4" s="28">
+      <c r="N4" s="38">
         <f>$N33/$D33</f>
         <v>0.46367107017331227</v>
       </c>
-      <c r="O4" s="28">
+      <c r="O4" s="38">
         <f>$N45/$D45</f>
         <v>0.45457034220532322</v>
       </c>
-      <c r="P4" s="28">
+      <c r="P4" s="38">
         <f>$N57/$D57</f>
         <v>0.46647167154154479</v>
       </c>
-      <c r="Q4" s="28">
+      <c r="Q4" s="38">
         <f>$N69/$D69</f>
         <v>0.47530777292849657</v>
       </c>
-      <c r="R4" s="28">
+      <c r="R4" s="38">
         <f>$N81/$D81</f>
         <v>0.47333726268767834</v>
       </c>
-      <c r="S4" s="28">
+      <c r="S4" s="38">
         <f>$N93/$D93</f>
         <v>0.4620528557687904</v>
       </c>
-      <c r="T4" s="28">
+      <c r="T4" s="38">
         <f>$N105/$D105</f>
         <v>0.46701562620275577</v>
       </c>
@@ -14709,71 +14719,71 @@
         <f t="shared" ref="B5:B15" si="8">B4*2</f>
         <v>2</v>
       </c>
-      <c r="C5" s="28">
+      <c r="C5" s="38">
         <f t="shared" si="0"/>
         <v>1.8298393973848777</v>
       </c>
-      <c r="D5" s="28">
+      <c r="D5" s="38">
         <f t="shared" si="1"/>
         <v>1.8602765510750743</v>
       </c>
-      <c r="E5" s="28">
+      <c r="E5" s="38">
         <f t="shared" si="2"/>
         <v>1.8388977985129027</v>
       </c>
-      <c r="F5" s="28">
+      <c r="F5" s="38">
         <f t="shared" si="3"/>
         <v>1.8891218776441157</v>
       </c>
-      <c r="G5" s="28">
+      <c r="G5" s="38">
         <f t="shared" si="4"/>
         <v>1.8450709296464318</v>
       </c>
-      <c r="H5" s="28">
+      <c r="H5" s="38">
         <f t="shared" si="5"/>
         <v>1.81163504968383</v>
       </c>
-      <c r="I5" s="28">
+      <c r="I5" s="38">
         <f t="shared" si="6"/>
         <v>1.9368389580296745</v>
       </c>
-      <c r="J5" s="28">
+      <c r="J5" s="38">
         <f t="shared" si="7"/>
         <v>1.9099374309900627</v>
       </c>
-      <c r="L5" s="31">
+      <c r="L5" s="30">
         <f t="shared" ref="L5:L15" si="9">L4*2</f>
         <v>2</v>
       </c>
-      <c r="M5" s="28">
+      <c r="M5" s="38">
         <f t="shared" ref="M5:M15" si="10">$N22/$D22</f>
         <v>0.54649604846696054</v>
       </c>
-      <c r="N5" s="28">
+      <c r="N5" s="38">
         <f t="shared" ref="N5:N15" si="11">$N34/$D34</f>
         <v>0.53755448318804488</v>
       </c>
-      <c r="O5" s="28">
+      <c r="O5" s="38">
         <f t="shared" ref="O5:O15" si="12">$N46/$D46</f>
         <v>0.54380401173392534</v>
       </c>
-      <c r="P5" s="28">
+      <c r="P5" s="38">
         <f t="shared" ref="P5:P15" si="13">$N58/$D58</f>
         <v>0.52934647141299274</v>
       </c>
-      <c r="Q5" s="28">
+      <c r="Q5" s="38">
         <f t="shared" ref="Q5:Q15" si="14">$N70/$D70</f>
         <v>0.54198458386184023</v>
       </c>
-      <c r="R5" s="28">
+      <c r="R5" s="38">
         <f t="shared" ref="R5:R15" si="15">$N82/$D82</f>
         <v>0.55198755410176115</v>
       </c>
-      <c r="S5" s="28">
+      <c r="S5" s="38">
         <f t="shared" ref="S5:S15" si="16">$N94/$D94</f>
         <v>0.51630518678604509</v>
       </c>
-      <c r="T5" s="28">
+      <c r="T5" s="38">
         <f t="shared" ref="T5:T15" si="17">$N106/$D106</f>
         <v>0.52357736110843467</v>
       </c>
@@ -14783,71 +14793,71 @@
         <f t="shared" si="8"/>
         <v>4</v>
       </c>
-      <c r="C6" s="28">
+      <c r="C6" s="38">
         <f t="shared" si="0"/>
         <v>1.4712727272727273</v>
       </c>
-      <c r="D6" s="28">
+      <c r="D6" s="38">
         <f t="shared" si="1"/>
         <v>1.5028947987761827</v>
       </c>
-      <c r="E6" s="28">
+      <c r="E6" s="38">
         <f t="shared" si="2"/>
         <v>1.5663340812526856</v>
       </c>
-      <c r="F6" s="28">
+      <c r="F6" s="38">
         <f t="shared" si="3"/>
         <v>1.5370088782067004</v>
       </c>
-      <c r="G6" s="28">
+      <c r="G6" s="38">
         <f t="shared" si="4"/>
         <v>1.562894775498213</v>
       </c>
-      <c r="H6" s="28">
+      <c r="H6" s="38">
         <f t="shared" si="5"/>
         <v>1.4900034218116047</v>
       </c>
-      <c r="I6" s="28">
+      <c r="I6" s="38">
         <f t="shared" si="6"/>
         <v>1.578177945590086</v>
       </c>
-      <c r="J6" s="28">
+      <c r="J6" s="38">
         <f t="shared" si="7"/>
         <v>1.5781752607466613</v>
       </c>
-      <c r="L6" s="31">
+      <c r="L6" s="30">
         <f t="shared" si="9"/>
         <v>4</v>
       </c>
-      <c r="M6" s="28">
+      <c r="M6" s="38">
         <f t="shared" si="10"/>
         <v>0.67968363816114685</v>
       </c>
-      <c r="N6" s="28">
+      <c r="N6" s="38">
         <f t="shared" si="11"/>
         <v>0.66538256757179992</v>
       </c>
-      <c r="O6" s="28">
+      <c r="O6" s="38">
         <f t="shared" si="12"/>
         <v>0.63843340444986274</v>
       </c>
-      <c r="P6" s="28">
+      <c r="P6" s="38">
         <f t="shared" si="13"/>
         <v>0.6506143290250519</v>
       </c>
-      <c r="Q6" s="28">
+      <c r="Q6" s="38">
         <f t="shared" si="14"/>
         <v>0.63983834080015034</v>
       </c>
-      <c r="R6" s="28">
+      <c r="R6" s="38">
         <f t="shared" si="15"/>
         <v>0.67113939831370362</v>
       </c>
-      <c r="S6" s="28">
+      <c r="S6" s="38">
         <f t="shared" si="16"/>
         <v>0.6336421078461445</v>
       </c>
-      <c r="T6" s="28">
+      <c r="T6" s="38">
         <f t="shared" si="17"/>
         <v>0.63364318581884449</v>
       </c>
@@ -14857,71 +14867,71 @@
         <f t="shared" si="8"/>
         <v>8</v>
       </c>
-      <c r="C7" s="28">
+      <c r="C7" s="38">
         <f t="shared" si="0"/>
         <v>1.1929850024189648</v>
       </c>
-      <c r="D7" s="28">
+      <c r="D7" s="38">
         <f t="shared" si="1"/>
         <v>1.2353275274517228</v>
       </c>
-      <c r="E7" s="28">
+      <c r="E7" s="38">
         <f t="shared" si="2"/>
         <v>1.2008062312107133</v>
       </c>
-      <c r="F7" s="28">
+      <c r="F7" s="38">
         <f t="shared" si="3"/>
         <v>1.2377442209976384</v>
       </c>
-      <c r="G7" s="28">
+      <c r="G7" s="38">
         <f t="shared" si="4"/>
         <v>1.2637135316356372</v>
       </c>
-      <c r="H7" s="28">
+      <c r="H7" s="38">
         <f t="shared" si="5"/>
         <v>1.2211225788208682</v>
       </c>
-      <c r="I7" s="28">
+      <c r="I7" s="38">
         <f t="shared" si="6"/>
         <v>1.2746239000851547</v>
       </c>
-      <c r="J7" s="28">
+      <c r="J7" s="38">
         <f t="shared" si="7"/>
         <v>1.2714788732394366</v>
       </c>
-      <c r="L7" s="31">
+      <c r="L7" s="30">
         <f t="shared" si="9"/>
         <v>8</v>
       </c>
-      <c r="M7" s="28">
+      <c r="M7" s="38">
         <f t="shared" si="10"/>
         <v>0.8382335050083134</v>
       </c>
-      <c r="N7" s="28">
+      <c r="N7" s="38">
         <f t="shared" si="11"/>
         <v>0.80950191570881225</v>
       </c>
-      <c r="O7" s="28">
+      <c r="O7" s="38">
         <f t="shared" si="12"/>
         <v>0.83277382645803688</v>
       </c>
-      <c r="P7" s="28">
+      <c r="P7" s="38">
         <f t="shared" si="13"/>
         <v>0.80792136455623009</v>
       </c>
-      <c r="Q7" s="28">
+      <c r="Q7" s="38">
         <f t="shared" si="14"/>
         <v>0.79131858207270278</v>
       </c>
-      <c r="R7" s="28">
+      <c r="R7" s="38">
         <f t="shared" si="15"/>
         <v>0.8189186059974527</v>
       </c>
-      <c r="S7" s="28">
+      <c r="S7" s="38">
         <f t="shared" si="16"/>
         <v>0.78454515087406751</v>
       </c>
-      <c r="T7" s="28">
+      <c r="T7" s="38">
         <f t="shared" si="17"/>
         <v>0.78648573802270838</v>
       </c>
@@ -14931,71 +14941,71 @@
         <f t="shared" si="8"/>
         <v>16</v>
       </c>
-      <c r="C8" s="28">
+      <c r="C8" s="38">
         <f t="shared" si="0"/>
         <v>1.0648171374103246</v>
       </c>
-      <c r="D8" s="28">
+      <c r="D8" s="38">
         <f t="shared" si="1"/>
         <v>0.83379851143009043</v>
       </c>
-      <c r="E8" s="28">
+      <c r="E8" s="38">
         <f t="shared" si="2"/>
         <v>0.92031080592699677</v>
       </c>
-      <c r="F8" s="28">
+      <c r="F8" s="38">
         <f t="shared" si="3"/>
         <v>1.046063377981052</v>
       </c>
-      <c r="G8" s="28">
+      <c r="G8" s="38">
         <f t="shared" si="4"/>
         <v>1.0826873385012921</v>
       </c>
-      <c r="H8" s="28">
+      <c r="H8" s="38">
         <f t="shared" si="5"/>
         <v>1.0187611361492506</v>
       </c>
-      <c r="I8" s="28">
+      <c r="I8" s="38">
         <f t="shared" si="6"/>
         <v>1.0292583120204604</v>
       </c>
-      <c r="J8" s="28">
+      <c r="J8" s="38">
         <f t="shared" si="7"/>
         <v>0.9094594594594595</v>
       </c>
-      <c r="L8" s="31">
+      <c r="L8" s="30">
         <f t="shared" si="9"/>
         <v>16</v>
       </c>
-      <c r="M8" s="28">
+      <c r="M8" s="38">
         <f t="shared" si="10"/>
         <v>0.9391283863368669</v>
       </c>
-      <c r="N8" s="28">
+      <c r="N8" s="38">
         <f t="shared" si="11"/>
         <v>1.1993305172551207</v>
       </c>
-      <c r="O8" s="28">
+      <c r="O8" s="38">
         <f t="shared" si="12"/>
         <v>1.086589436481445</v>
       </c>
-      <c r="P8" s="28">
+      <c r="P8" s="38">
         <f t="shared" si="13"/>
         <v>0.95596502186133658</v>
       </c>
-      <c r="Q8" s="28">
+      <c r="Q8" s="38">
         <f t="shared" si="14"/>
         <v>0.92362768496420045</v>
       </c>
-      <c r="R8" s="28">
+      <c r="R8" s="38">
         <f t="shared" si="15"/>
         <v>0.98158436213991773</v>
       </c>
-      <c r="S8" s="28">
+      <c r="S8" s="38">
         <f t="shared" si="16"/>
         <v>0.97157340224629751</v>
       </c>
-      <c r="T8" s="28">
+      <c r="T8" s="38">
         <f t="shared" si="17"/>
         <v>1.0995542347696881</v>
       </c>
@@ -15005,71 +15015,71 @@
         <f t="shared" si="8"/>
         <v>32</v>
       </c>
-      <c r="C9" s="28">
+      <c r="C9" s="38">
         <f t="shared" si="0"/>
         <v>1.0087624349260347</v>
       </c>
-      <c r="D9" s="28">
+      <c r="D9" s="38">
         <f t="shared" si="1"/>
         <v>0.93242148834698113</v>
       </c>
-      <c r="E9" s="28">
+      <c r="E9" s="38">
         <f t="shared" si="2"/>
         <v>0.9526691683815518</v>
       </c>
-      <c r="F9" s="28">
+      <c r="F9" s="38">
         <f t="shared" si="3"/>
         <v>0.92719188550785037</v>
       </c>
-      <c r="G9" s="28">
+      <c r="G9" s="38">
         <f t="shared" si="4"/>
         <v>0.94266441821247882</v>
       </c>
-      <c r="H9" s="28">
+      <c r="H9" s="38">
         <f t="shared" si="5"/>
         <v>0.86587942821628339</v>
       </c>
-      <c r="I9" s="28">
+      <c r="I9" s="38">
         <f t="shared" si="6"/>
         <v>0.85474353154788929</v>
       </c>
-      <c r="J9" s="28">
+      <c r="J9" s="38">
         <f t="shared" si="7"/>
         <v>0.69172609330698509</v>
       </c>
-      <c r="L9" s="31">
+      <c r="L9" s="30">
         <f t="shared" si="9"/>
         <v>32</v>
       </c>
-      <c r="M9" s="28">
+      <c r="M9" s="38">
         <f t="shared" si="10"/>
         <v>0.9913136784017168</v>
       </c>
-      <c r="N9" s="28">
+      <c r="N9" s="38">
         <f t="shared" si="11"/>
         <v>1.0724763559158463</v>
       </c>
-      <c r="O9" s="28">
+      <c r="O9" s="38">
         <f t="shared" si="12"/>
         <v>1.0496823379923761</v>
       </c>
-      <c r="P9" s="28">
+      <c r="P9" s="38">
         <f t="shared" si="13"/>
         <v>1.0785254008691745</v>
       </c>
-      <c r="Q9" s="28">
+      <c r="Q9" s="38">
         <f t="shared" si="14"/>
         <v>1.0608228980322005</v>
       </c>
-      <c r="R9" s="28">
+      <c r="R9" s="38">
         <f t="shared" si="15"/>
         <v>1.1548952052828021</v>
       </c>
-      <c r="S9" s="28">
+      <c r="S9" s="38">
         <f t="shared" si="16"/>
         <v>1.1699415825809878</v>
       </c>
-      <c r="T9" s="28">
+      <c r="T9" s="38">
         <f t="shared" si="17"/>
         <v>1.4456589243572229</v>
       </c>
@@ -15079,71 +15089,71 @@
         <f t="shared" si="8"/>
         <v>64</v>
       </c>
-      <c r="C10" s="28">
+      <c r="C10" s="38">
         <f t="shared" si="0"/>
         <v>0.91525340652877163</v>
       </c>
-      <c r="D10" s="28">
+      <c r="D10" s="38">
         <f t="shared" si="1"/>
         <v>0.8761198081621574</v>
       </c>
-      <c r="E10" s="28">
+      <c r="E10" s="38">
         <f t="shared" si="2"/>
         <v>0.87770717157307732</v>
       </c>
-      <c r="F10" s="28">
+      <c r="F10" s="38">
         <f t="shared" si="3"/>
         <v>0.83776511554289335</v>
       </c>
-      <c r="G10" s="28">
+      <c r="G10" s="38">
         <f t="shared" si="4"/>
         <v>0.9425535191744957</v>
       </c>
-      <c r="H10" s="28">
+      <c r="H10" s="38">
         <f t="shared" si="5"/>
         <v>0.83068135454916359</v>
       </c>
-      <c r="I10" s="28">
+      <c r="I10" s="38">
         <f t="shared" si="6"/>
         <v>0.79136104319478406</v>
       </c>
-      <c r="J10" s="28">
+      <c r="J10" s="38">
         <f t="shared" si="7"/>
         <v>0.69221556886227553</v>
       </c>
-      <c r="L10" s="31">
+      <c r="L10" s="30">
         <f t="shared" si="9"/>
         <v>64</v>
       </c>
-      <c r="M10" s="28">
+      <c r="M10" s="38">
         <f t="shared" si="10"/>
         <v>1.092593584319606</v>
       </c>
-      <c r="N10" s="28">
+      <c r="N10" s="38">
         <f t="shared" si="11"/>
         <v>1.1413964057013013</v>
       </c>
-      <c r="O10" s="28">
+      <c r="O10" s="38">
         <f t="shared" si="12"/>
         <v>1.1393321513002366</v>
       </c>
-      <c r="P10" s="28">
+      <c r="P10" s="38">
         <f t="shared" si="13"/>
         <v>1.1936519931985641</v>
       </c>
-      <c r="Q10" s="28">
+      <c r="Q10" s="38">
         <f t="shared" si="14"/>
         <v>1.0609477124183007</v>
       </c>
-      <c r="R10" s="28">
+      <c r="R10" s="38">
         <f t="shared" si="15"/>
         <v>1.2038310412573674</v>
       </c>
-      <c r="S10" s="28">
+      <c r="S10" s="38">
         <f t="shared" si="16"/>
         <v>1.2636457260556127</v>
       </c>
-      <c r="T10" s="28">
+      <c r="T10" s="38">
         <f t="shared" si="17"/>
         <v>1.4446366782006919</v>
       </c>
@@ -15153,71 +15163,71 @@
         <f t="shared" si="8"/>
         <v>128</v>
       </c>
-      <c r="C11" s="28">
+      <c r="C11" s="38">
         <f t="shared" si="0"/>
         <v>0.8754909090909091</v>
       </c>
-      <c r="D11" s="28">
+      <c r="D11" s="38">
         <f t="shared" si="1"/>
         <v>0.89186946902654873</v>
       </c>
-      <c r="E11" s="28">
+      <c r="E11" s="38">
         <f t="shared" si="2"/>
         <v>0.86240233081711037</v>
       </c>
-      <c r="F11" s="28">
+      <c r="F11" s="38">
         <f t="shared" si="3"/>
         <v>0.8178237321516495</v>
       </c>
-      <c r="G11" s="28">
+      <c r="G11" s="38">
         <f t="shared" si="4"/>
         <v>0.86517571884984035</v>
       </c>
-      <c r="H11" s="28">
+      <c r="H11" s="38">
         <f t="shared" si="5"/>
         <v>0.81315565636518294</v>
       </c>
-      <c r="I11" s="28">
+      <c r="I11" s="38">
         <f t="shared" si="6"/>
         <v>0.75804195804195806</v>
       </c>
-      <c r="J11" s="28">
+      <c r="J11" s="38">
         <f t="shared" si="7"/>
         <v>0.67375949143563485</v>
       </c>
-      <c r="L11" s="31">
+      <c r="L11" s="30">
         <f t="shared" si="9"/>
         <v>128</v>
       </c>
-      <c r="M11" s="28">
+      <c r="M11" s="38">
         <f t="shared" si="10"/>
         <v>1.142216315002492</v>
       </c>
-      <c r="N11" s="28">
+      <c r="N11" s="38">
         <f t="shared" si="11"/>
         <v>1.1212403100775192</v>
       </c>
-      <c r="O11" s="28">
+      <c r="O11" s="38">
         <f t="shared" si="12"/>
         <v>1.159551597051597</v>
       </c>
-      <c r="P11" s="28">
+      <c r="P11" s="38">
         <f t="shared" si="13"/>
         <v>1.2227573750752558</v>
       </c>
-      <c r="Q11" s="28">
+      <c r="Q11" s="38">
         <f t="shared" si="14"/>
         <v>1.1558345642540619</v>
       </c>
-      <c r="R11" s="28">
+      <c r="R11" s="38">
         <f t="shared" si="15"/>
         <v>1.2297768479776847</v>
       </c>
-      <c r="S11" s="28">
+      <c r="S11" s="38">
         <f t="shared" si="16"/>
         <v>1.3191881918819188</v>
       </c>
-      <c r="T11" s="37">
+      <c r="T11" s="39">
         <f t="shared" si="17"/>
         <v>1.4842091469007992</v>
       </c>
@@ -15227,71 +15237,71 @@
         <f t="shared" si="8"/>
         <v>256</v>
       </c>
-      <c r="C12" s="28">
+      <c r="C12" s="38">
         <f t="shared" si="0"/>
         <v>0.86047918120493139</v>
       </c>
-      <c r="D12" s="28">
+      <c r="D12" s="38">
         <f t="shared" si="1"/>
         <v>0.88860621479193169</v>
       </c>
-      <c r="E12" s="28">
+      <c r="E12" s="38">
         <f t="shared" si="2"/>
         <v>0.85033146353901068</v>
       </c>
-      <c r="F12" s="28">
+      <c r="F12" s="38">
         <f t="shared" si="3"/>
         <v>0.86423505572441739</v>
       </c>
-      <c r="G12" s="28">
+      <c r="G12" s="38">
         <f t="shared" si="4"/>
         <v>0.83931333127126517</v>
       </c>
-      <c r="H12" s="28">
+      <c r="H12" s="38">
         <f t="shared" si="5"/>
         <v>0.83637122582440515</v>
       </c>
-      <c r="I12" s="28">
+      <c r="I12" s="38">
         <f t="shared" si="6"/>
         <v>0.78081546075889696</v>
       </c>
-      <c r="J12" s="28">
+      <c r="J12" s="38">
         <f t="shared" si="7"/>
         <v>0.6780991006877094</v>
       </c>
-      <c r="L12" s="31">
+      <c r="L12" s="30">
         <f t="shared" si="9"/>
         <v>256</v>
       </c>
-      <c r="M12" s="28">
+      <c r="M12" s="38">
         <f t="shared" si="10"/>
         <v>1.1621431660899655</v>
       </c>
-      <c r="N12" s="28">
+      <c r="N12" s="38">
         <f t="shared" si="11"/>
         <v>1.125357873210634</v>
       </c>
-      <c r="O12" s="28">
+      <c r="O12" s="38">
         <f t="shared" si="12"/>
         <v>1.1760119940029985</v>
       </c>
-      <c r="P12" s="28">
+      <c r="P12" s="38">
         <f t="shared" si="13"/>
         <v>1.157092614302462</v>
       </c>
-      <c r="Q12" s="28">
+      <c r="Q12" s="38">
         <f t="shared" si="14"/>
         <v>1.1914501566242859</v>
       </c>
-      <c r="R12" s="28">
+      <c r="R12" s="38">
         <f t="shared" si="15"/>
         <v>1.1956413242388955</v>
       </c>
-      <c r="S12" s="28">
+      <c r="S12" s="38">
         <f t="shared" si="16"/>
         <v>1.2807123453063689</v>
       </c>
-      <c r="T12" s="28">
+      <c r="T12" s="38">
         <f t="shared" si="17"/>
         <v>1.4747107008191394</v>
       </c>
@@ -15301,71 +15311,71 @@
         <f t="shared" si="8"/>
         <v>512</v>
       </c>
-      <c r="C13" s="28">
+      <c r="C13" s="38">
         <f t="shared" si="0"/>
         <v>0.92405063291139256</v>
       </c>
-      <c r="D13" s="28">
+      <c r="D13" s="38">
         <f t="shared" si="1"/>
         <v>0.97586322494133426</v>
       </c>
-      <c r="E13" s="28">
+      <c r="E13" s="38">
         <f t="shared" si="2"/>
         <v>0.93642713389369003</v>
       </c>
-      <c r="F13" s="28">
+      <c r="F13" s="38">
         <f t="shared" si="3"/>
         <v>1.0083981337480559</v>
       </c>
-      <c r="G13" s="28">
+      <c r="G13" s="38">
         <f t="shared" si="4"/>
         <v>1.0217199882594659</v>
       </c>
-      <c r="H13" s="28">
+      <c r="H13" s="38">
         <f t="shared" si="5"/>
         <v>0.95464882943143814</v>
       </c>
-      <c r="I13" s="28">
+      <c r="I13" s="38">
         <f t="shared" si="6"/>
         <v>0.89207650273224048</v>
       </c>
-      <c r="J13" s="28">
+      <c r="J13" s="38">
         <f t="shared" si="7"/>
         <v>0.7628310898827616</v>
       </c>
-      <c r="L13" s="31">
+      <c r="L13" s="30">
         <f t="shared" si="9"/>
         <v>512</v>
       </c>
-      <c r="M13" s="28">
+      <c r="M13" s="38">
         <f t="shared" si="10"/>
         <v>1.0821917808219177</v>
       </c>
-      <c r="N13" s="28">
+      <c r="N13" s="38">
         <f t="shared" si="11"/>
         <v>1.0247337684644451</v>
       </c>
-      <c r="O13" s="28">
+      <c r="O13" s="38">
         <f t="shared" si="12"/>
         <v>1.0678887484197219</v>
       </c>
-      <c r="P13" s="28">
+      <c r="P13" s="38">
         <f t="shared" si="13"/>
         <v>0.99167180752621842</v>
       </c>
-      <c r="Q13" s="28">
+      <c r="Q13" s="38">
         <f t="shared" si="14"/>
         <v>0.97874174087905763</v>
       </c>
-      <c r="R13" s="28">
+      <c r="R13" s="38">
         <f t="shared" si="15"/>
         <v>1.047505605381166</v>
       </c>
-      <c r="S13" s="28">
+      <c r="S13" s="38">
         <f t="shared" si="16"/>
         <v>1.1209800918836141</v>
       </c>
-      <c r="T13" s="28">
+      <c r="T13" s="38">
         <f t="shared" si="17"/>
         <v>1.3109061930783243</v>
       </c>
@@ -15375,71 +15385,71 @@
         <f t="shared" si="8"/>
         <v>1024</v>
       </c>
-      <c r="C14" s="28">
+      <c r="C14" s="38">
         <f t="shared" si="0"/>
         <v>1.2790811707905854</v>
       </c>
-      <c r="D14" s="28">
+      <c r="D14" s="38">
         <f t="shared" si="1"/>
         <v>1.3597809296447128</v>
       </c>
-      <c r="E14" s="28">
+      <c r="E14" s="38">
         <f t="shared" si="2"/>
         <v>1.5360233447373717</v>
       </c>
-      <c r="F14" s="28">
+      <c r="F14" s="38">
         <f t="shared" si="3"/>
         <v>1.7487666034155598</v>
       </c>
-      <c r="G14" s="28">
+      <c r="G14" s="38">
         <f t="shared" si="4"/>
         <v>1.7106668322364336</v>
       </c>
-      <c r="H14" s="28">
+      <c r="H14" s="38">
         <f t="shared" si="5"/>
         <v>1.5718976449275361</v>
       </c>
-      <c r="I14" s="28">
+      <c r="I14" s="38">
         <f t="shared" si="6"/>
         <v>1.2979189485213583</v>
       </c>
-      <c r="J14" s="28">
+      <c r="J14" s="38">
         <f t="shared" si="7"/>
         <v>1.1875</v>
       </c>
-      <c r="L14" s="31">
+      <c r="L14" s="30">
         <f t="shared" si="9"/>
         <v>1024</v>
       </c>
-      <c r="M14" s="28">
+      <c r="M14" s="38">
         <f t="shared" si="10"/>
         <v>0.78181121170121781</v>
       </c>
-      <c r="N14" s="28">
+      <c r="N14" s="38">
         <f t="shared" si="11"/>
         <v>0.73541257874625643</v>
       </c>
-      <c r="O14" s="28">
+      <c r="O14" s="38">
         <f t="shared" si="12"/>
         <v>0.65103177202751394</v>
       </c>
-      <c r="P14" s="28">
+      <c r="P14" s="38">
         <f t="shared" si="13"/>
         <v>0.57183159722222221</v>
       </c>
-      <c r="Q14" s="28">
+      <c r="Q14" s="38">
         <f t="shared" si="14"/>
         <v>0.58456736353077821</v>
       </c>
-      <c r="R14" s="28">
+      <c r="R14" s="38">
         <f t="shared" si="15"/>
         <v>0.63617373766476992</v>
       </c>
-      <c r="S14" s="28">
+      <c r="S14" s="38">
         <f t="shared" si="16"/>
         <v>0.77046413502109701</v>
       </c>
-      <c r="T14" s="28">
+      <c r="T14" s="38">
         <f t="shared" si="17"/>
         <v>0.84210526315789469</v>
       </c>
@@ -15449,71 +15459,71 @@
         <f t="shared" si="8"/>
         <v>2048</v>
       </c>
-      <c r="C15" s="28">
+      <c r="C15" s="38">
         <f t="shared" si="0"/>
         <v>2.224679735765291</v>
       </c>
-      <c r="D15" s="28">
+      <c r="D15" s="38">
         <f t="shared" si="1"/>
         <v>2.7255841548010227</v>
       </c>
-      <c r="E15" s="28">
+      <c r="E15" s="38">
         <f t="shared" si="2"/>
         <v>3.0606265772142551</v>
       </c>
-      <c r="F15" s="28">
+      <c r="F15" s="38">
         <f t="shared" si="3"/>
         <v>3.5879996977253836</v>
       </c>
-      <c r="G15" s="37">
+      <c r="G15" s="39">
         <f t="shared" si="4"/>
         <v>3.8726644685193907</v>
       </c>
-      <c r="H15" s="28">
+      <c r="H15" s="38">
         <f t="shared" si="5"/>
         <v>3.5434412265758093</v>
       </c>
-      <c r="I15" s="28">
+      <c r="I15" s="38">
         <f t="shared" si="6"/>
         <v>3.3803819322105566</v>
       </c>
-      <c r="J15" s="28">
+      <c r="J15" s="38">
         <f t="shared" si="7"/>
         <v>2.5675852627819773</v>
       </c>
-      <c r="L15" s="31">
+      <c r="L15" s="30">
         <f t="shared" si="9"/>
         <v>2048</v>
       </c>
-      <c r="M15" s="28">
+      <c r="M15" s="38">
         <f t="shared" si="10"/>
         <v>0.44950290323744035</v>
       </c>
-      <c r="N15" s="28">
+      <c r="N15" s="38">
         <f t="shared" si="11"/>
         <v>0.36689382649900371</v>
       </c>
-      <c r="O15" s="28">
+      <c r="O15" s="38">
         <f t="shared" si="12"/>
         <v>0.32673048304709806</v>
       </c>
-      <c r="P15" s="28">
+      <c r="P15" s="38">
         <f t="shared" si="13"/>
         <v>0.27870682392586349</v>
       </c>
-      <c r="Q15" s="28">
+      <c r="Q15" s="38">
         <f t="shared" si="14"/>
         <v>0.25822015001013582</v>
       </c>
-      <c r="R15" s="28">
+      <c r="R15" s="38">
         <f t="shared" si="15"/>
         <v>0.28221153846153846</v>
       </c>
-      <c r="S15" s="28">
+      <c r="S15" s="38">
         <f t="shared" si="16"/>
         <v>0.29582456067207269</v>
       </c>
-      <c r="T15" s="28">
+      <c r="T15" s="38">
         <f t="shared" si="17"/>
         <v>0.38947100004636281</v>
       </c>
@@ -15539,52 +15549,52 @@
       <c r="S18" s="3"/>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="B19" s="32" t="s">
+      <c r="B19" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C19" s="33" t="s">
+      <c r="C19" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="D19" s="34" t="s">
+      <c r="D19" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="E19" s="35" t="s">
+      <c r="E19" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="F19" s="35" t="s">
+      <c r="F19" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="G19" s="35" t="s">
+      <c r="G19" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="H19" s="35" t="s">
+      <c r="H19" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="I19" s="35" t="s">
+      <c r="I19" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="L19" s="32" t="s">
+      <c r="L19" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="M19" s="33" t="s">
+      <c r="M19" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="N19" s="36" t="s">
+      <c r="N19" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="O19" s="35" t="s">
+      <c r="O19" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="P19" s="35" t="s">
+      <c r="P19" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="Q19" s="35" t="s">
+      <c r="Q19" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="R19" s="35" t="s">
+      <c r="R19" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="S19" s="35" t="s">
+      <c r="S19" s="34" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated comment and image
</commit_message>
<xml_diff>
--- a/docs/Comparison.xlsx
+++ b/docs/Comparison.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7452" yWindow="0" windowWidth="22110" windowHeight="9402" activeTab="3"/>
+    <workbookView xWindow="8394" yWindow="0" windowWidth="22110" windowHeight="9402"/>
   </bookViews>
   <sheets>
     <sheet name="Graphs" sheetId="4" r:id="rId1"/>
@@ -75,9 +75,6 @@
     <t>TBB Execution Time Records</t>
   </si>
   <si>
-    <t>Tiles</t>
-  </si>
-  <si>
     <t>Ratio</t>
   </si>
   <si>
@@ -100,6 +97,9 @@
   </si>
   <si>
     <t>C++ Speed Up</t>
+  </si>
+  <si>
+    <t>VP</t>
   </si>
 </sst>
 </file>
@@ -220,7 +220,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -262,14 +261,15 @@
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -11972,9 +11972,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A72" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C102" sqref="C102"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData/>
@@ -11987,9 +11985,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:W116"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -12016,10 +12012,10 @@
       <c r="B5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="36"/>
+      <c r="D5" s="37"/>
     </row>
     <row r="6" spans="2:23" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" s="13" t="s">
@@ -12519,27 +12515,27 @@
       <c r="D19" s="11"/>
     </row>
     <row r="20" spans="2:10" ht="25.8" x14ac:dyDescent="0.95">
-      <c r="B20" s="17" t="s">
-        <v>17</v>
+      <c r="B20" s="16" t="s">
+        <v>16</v>
       </c>
       <c r="C20" s="11"/>
       <c r="D20" s="11"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B22" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="D22" s="36"/>
+      <c r="D22" s="37"/>
       <c r="E22"/>
       <c r="F22"/>
       <c r="G22"/>
-      <c r="H22" s="37" t="s">
+      <c r="H22" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I22" s="37"/>
+      <c r="I22" s="38"/>
       <c r="J22" s="5">
         <f>'Execution Time Records'!D20</f>
         <v>12455</v>
@@ -12549,28 +12545,28 @@
       <c r="B23" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C23" s="18">
+      <c r="C23" s="17">
         <v>1</v>
       </c>
       <c r="D23" s="12">
         <v>2</v>
       </c>
-      <c r="E23" s="19">
+      <c r="E23" s="18">
         <v>3</v>
       </c>
-      <c r="F23" s="19">
+      <c r="F23" s="18">
         <v>4</v>
       </c>
-      <c r="G23" s="19">
+      <c r="G23" s="18">
         <v>5</v>
       </c>
-      <c r="H23" s="19">
+      <c r="H23" s="18">
         <v>6</v>
       </c>
-      <c r="I23" s="19">
+      <c r="I23" s="18">
         <v>7</v>
       </c>
-      <c r="J23" s="19">
+      <c r="J23" s="18">
         <v>8</v>
       </c>
     </row>
@@ -13449,9 +13445,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -13460,7 +13454,7 @@
   <sheetData>
     <row r="2" spans="2:10" ht="25.8" x14ac:dyDescent="0.95">
       <c r="B2" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
@@ -13500,10 +13494,10 @@
       <c r="B5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="36"/>
+      <c r="D5" s="37"/>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
@@ -13996,8 +13990,8 @@
       </c>
     </row>
     <row r="20" spans="2:10" ht="25.8" x14ac:dyDescent="0.95">
-      <c r="B20" s="17" t="s">
-        <v>22</v>
+      <c r="B20" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C20" s="11"/>
       <c r="D20" s="11"/>
@@ -14020,16 +14014,16 @@
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B22" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="D22" s="36"/>
-      <c r="H22" s="37" t="s">
+      <c r="D22" s="37"/>
+      <c r="H22" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I22" s="37"/>
+      <c r="I22" s="38"/>
       <c r="J22" s="5">
         <f>'Execution Time Records'!N20</f>
         <v>5993.2</v>
@@ -14039,28 +14033,28 @@
       <c r="B23" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C23" s="18">
+      <c r="C23" s="17">
         <v>1</v>
       </c>
       <c r="D23" s="12">
         <v>2</v>
       </c>
-      <c r="E23" s="19">
+      <c r="E23" s="18">
         <v>3</v>
       </c>
-      <c r="F23" s="19">
+      <c r="F23" s="18">
         <v>4</v>
       </c>
-      <c r="G23" s="19">
+      <c r="G23" s="18">
         <v>5</v>
       </c>
-      <c r="H23" s="19">
+      <c r="H23" s="18">
         <v>6</v>
       </c>
-      <c r="I23" s="19">
+      <c r="I23" s="18">
         <v>7</v>
       </c>
-      <c r="J23" s="19">
+      <c r="J23" s="18">
         <v>8</v>
       </c>
     </row>
@@ -14533,9 +14527,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:T116"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -14543,7 +14535,7 @@
     <col min="5" max="9" width="8.578125" style="3" customWidth="1"/>
     <col min="11" max="11" width="8.9453125" customWidth="1"/>
     <col min="12" max="12" width="11.578125" customWidth="1"/>
-    <col min="13" max="13" width="8.578125" style="26" customWidth="1"/>
+    <col min="13" max="13" width="8.578125" style="25" customWidth="1"/>
     <col min="14" max="18" width="8.578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -14559,10 +14551,10 @@
       <c r="J1" s="2"/>
     </row>
     <row r="2" spans="2:20" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="16" t="s">
+      <c r="B2" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="39" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="2"/>
@@ -14572,10 +14564,10 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
-      <c r="L2" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="M2" s="16" t="s">
+      <c r="L2" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" s="39" t="s">
         <v>10</v>
       </c>
       <c r="N2" s="2"/>
@@ -14587,58 +14579,58 @@
       <c r="T2" s="2"/>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.55000000000000004">
-      <c r="B3" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="29">
+      <c r="B3" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="19">
         <v>1</v>
       </c>
-      <c r="D3" s="29">
+      <c r="D3" s="19">
         <v>2</v>
       </c>
-      <c r="E3" s="29">
+      <c r="E3" s="19">
         <v>3</v>
       </c>
-      <c r="F3" s="29">
+      <c r="F3" s="19">
         <v>4</v>
       </c>
-      <c r="G3" s="29">
+      <c r="G3" s="19">
         <v>5</v>
       </c>
-      <c r="H3" s="29">
+      <c r="H3" s="19">
         <v>6</v>
       </c>
-      <c r="I3" s="29">
+      <c r="I3" s="19">
         <v>7</v>
       </c>
-      <c r="J3" s="29">
+      <c r="J3" s="19">
         <v>8</v>
       </c>
-      <c r="L3" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="M3" s="29">
+      <c r="L3" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" s="28">
         <v>1</v>
       </c>
-      <c r="N3" s="29">
+      <c r="N3" s="28">
         <v>2</v>
       </c>
-      <c r="O3" s="29">
+      <c r="O3" s="28">
         <v>3</v>
       </c>
-      <c r="P3" s="29">
+      <c r="P3" s="28">
         <v>4</v>
       </c>
-      <c r="Q3" s="29">
+      <c r="Q3" s="28">
         <v>5</v>
       </c>
-      <c r="R3" s="29">
+      <c r="R3" s="28">
         <v>6</v>
       </c>
-      <c r="S3" s="29">
+      <c r="S3" s="28">
         <v>7</v>
       </c>
-      <c r="T3" s="29">
+      <c r="T3" s="28">
         <v>8</v>
       </c>
     </row>
@@ -14646,70 +14638,70 @@
       <c r="B4" s="15">
         <v>1</v>
       </c>
-      <c r="C4" s="38">
+      <c r="C4" s="35">
         <f t="shared" ref="C4:C15" si="0">$D21/$N21</f>
         <v>2.1350202563591685</v>
       </c>
-      <c r="D4" s="38">
+      <c r="D4" s="35">
         <f t="shared" ref="D4:D15" si="1">$D33/$N33</f>
         <v>2.1567013003986149</v>
       </c>
-      <c r="E4" s="38">
+      <c r="E4" s="35">
         <f t="shared" ref="E4:E15" si="2">$D45/$N45</f>
         <v>2.199879550321199</v>
       </c>
-      <c r="F4" s="38">
+      <c r="F4" s="35">
         <f t="shared" ref="F4:F15" si="3">$D57/$N57</f>
         <v>2.1437529029261495</v>
       </c>
-      <c r="G4" s="38">
+      <c r="G4" s="35">
         <f t="shared" ref="G4:G15" si="4">$D69/$N69</f>
         <v>2.1038999506335361</v>
       </c>
-      <c r="H4" s="38">
+      <c r="H4" s="35">
         <f t="shared" ref="H4:H15" si="5">$D81/$N81</f>
         <v>2.1126585182029687</v>
       </c>
-      <c r="I4" s="38">
+      <c r="I4" s="35">
         <f t="shared" ref="I4:I15" si="6">$D93/$N93</f>
         <v>2.1642545598731164</v>
       </c>
-      <c r="J4" s="38">
+      <c r="J4" s="35">
         <f t="shared" ref="J4:J15" si="7">$D105/$N105</f>
         <v>2.1412559749464317</v>
       </c>
-      <c r="L4" s="30">
+      <c r="L4" s="29">
         <v>1</v>
       </c>
-      <c r="M4" s="38">
+      <c r="M4" s="35">
         <f>$N21/$D21</f>
         <v>0.46837963106977326</v>
       </c>
-      <c r="N4" s="38">
+      <c r="N4" s="35">
         <f>$N33/$D33</f>
         <v>0.46367107017331227</v>
       </c>
-      <c r="O4" s="38">
+      <c r="O4" s="35">
         <f>$N45/$D45</f>
         <v>0.45457034220532322</v>
       </c>
-      <c r="P4" s="38">
+      <c r="P4" s="35">
         <f>$N57/$D57</f>
         <v>0.46647167154154479</v>
       </c>
-      <c r="Q4" s="38">
+      <c r="Q4" s="35">
         <f>$N69/$D69</f>
         <v>0.47530777292849657</v>
       </c>
-      <c r="R4" s="38">
+      <c r="R4" s="35">
         <f>$N81/$D81</f>
         <v>0.47333726268767834</v>
       </c>
-      <c r="S4" s="38">
+      <c r="S4" s="35">
         <f>$N93/$D93</f>
         <v>0.4620528557687904</v>
       </c>
-      <c r="T4" s="38">
+      <c r="T4" s="35">
         <f>$N105/$D105</f>
         <v>0.46701562620275577</v>
       </c>
@@ -14719,71 +14711,71 @@
         <f t="shared" ref="B5:B15" si="8">B4*2</f>
         <v>2</v>
       </c>
-      <c r="C5" s="38">
+      <c r="C5" s="35">
         <f t="shared" si="0"/>
         <v>1.8298393973848777</v>
       </c>
-      <c r="D5" s="38">
+      <c r="D5" s="35">
         <f t="shared" si="1"/>
         <v>1.8602765510750743</v>
       </c>
-      <c r="E5" s="38">
+      <c r="E5" s="35">
         <f t="shared" si="2"/>
         <v>1.8388977985129027</v>
       </c>
-      <c r="F5" s="38">
+      <c r="F5" s="35">
         <f t="shared" si="3"/>
         <v>1.8891218776441157</v>
       </c>
-      <c r="G5" s="38">
+      <c r="G5" s="35">
         <f t="shared" si="4"/>
         <v>1.8450709296464318</v>
       </c>
-      <c r="H5" s="38">
+      <c r="H5" s="35">
         <f t="shared" si="5"/>
         <v>1.81163504968383</v>
       </c>
-      <c r="I5" s="38">
+      <c r="I5" s="35">
         <f t="shared" si="6"/>
         <v>1.9368389580296745</v>
       </c>
-      <c r="J5" s="38">
+      <c r="J5" s="35">
         <f t="shared" si="7"/>
         <v>1.9099374309900627</v>
       </c>
-      <c r="L5" s="30">
+      <c r="L5" s="29">
         <f t="shared" ref="L5:L15" si="9">L4*2</f>
         <v>2</v>
       </c>
-      <c r="M5" s="38">
+      <c r="M5" s="35">
         <f t="shared" ref="M5:M15" si="10">$N22/$D22</f>
         <v>0.54649604846696054</v>
       </c>
-      <c r="N5" s="38">
+      <c r="N5" s="35">
         <f t="shared" ref="N5:N15" si="11">$N34/$D34</f>
         <v>0.53755448318804488</v>
       </c>
-      <c r="O5" s="38">
+      <c r="O5" s="35">
         <f t="shared" ref="O5:O15" si="12">$N46/$D46</f>
         <v>0.54380401173392534</v>
       </c>
-      <c r="P5" s="38">
+      <c r="P5" s="35">
         <f t="shared" ref="P5:P15" si="13">$N58/$D58</f>
         <v>0.52934647141299274</v>
       </c>
-      <c r="Q5" s="38">
+      <c r="Q5" s="35">
         <f t="shared" ref="Q5:Q15" si="14">$N70/$D70</f>
         <v>0.54198458386184023</v>
       </c>
-      <c r="R5" s="38">
+      <c r="R5" s="35">
         <f t="shared" ref="R5:R15" si="15">$N82/$D82</f>
         <v>0.55198755410176115</v>
       </c>
-      <c r="S5" s="38">
+      <c r="S5" s="35">
         <f t="shared" ref="S5:S15" si="16">$N94/$D94</f>
         <v>0.51630518678604509</v>
       </c>
-      <c r="T5" s="38">
+      <c r="T5" s="35">
         <f t="shared" ref="T5:T15" si="17">$N106/$D106</f>
         <v>0.52357736110843467</v>
       </c>
@@ -14793,71 +14785,71 @@
         <f t="shared" si="8"/>
         <v>4</v>
       </c>
-      <c r="C6" s="38">
-        <f t="shared" si="0"/>
+      <c r="C6" s="35">
+        <f>$D23/$N23</f>
         <v>1.4712727272727273</v>
       </c>
-      <c r="D6" s="38">
+      <c r="D6" s="35">
         <f t="shared" si="1"/>
         <v>1.5028947987761827</v>
       </c>
-      <c r="E6" s="38">
+      <c r="E6" s="35">
         <f t="shared" si="2"/>
         <v>1.5663340812526856</v>
       </c>
-      <c r="F6" s="38">
+      <c r="F6" s="35">
         <f t="shared" si="3"/>
         <v>1.5370088782067004</v>
       </c>
-      <c r="G6" s="38">
+      <c r="G6" s="35">
         <f t="shared" si="4"/>
         <v>1.562894775498213</v>
       </c>
-      <c r="H6" s="38">
+      <c r="H6" s="35">
         <f t="shared" si="5"/>
         <v>1.4900034218116047</v>
       </c>
-      <c r="I6" s="38">
+      <c r="I6" s="35">
         <f t="shared" si="6"/>
         <v>1.578177945590086</v>
       </c>
-      <c r="J6" s="38">
+      <c r="J6" s="35">
         <f t="shared" si="7"/>
         <v>1.5781752607466613</v>
       </c>
-      <c r="L6" s="30">
+      <c r="L6" s="29">
         <f t="shared" si="9"/>
         <v>4</v>
       </c>
-      <c r="M6" s="38">
+      <c r="M6" s="35">
         <f t="shared" si="10"/>
         <v>0.67968363816114685</v>
       </c>
-      <c r="N6" s="38">
+      <c r="N6" s="35">
         <f t="shared" si="11"/>
         <v>0.66538256757179992</v>
       </c>
-      <c r="O6" s="38">
+      <c r="O6" s="35">
         <f t="shared" si="12"/>
         <v>0.63843340444986274</v>
       </c>
-      <c r="P6" s="38">
+      <c r="P6" s="35">
         <f t="shared" si="13"/>
         <v>0.6506143290250519</v>
       </c>
-      <c r="Q6" s="38">
+      <c r="Q6" s="35">
         <f t="shared" si="14"/>
         <v>0.63983834080015034</v>
       </c>
-      <c r="R6" s="38">
+      <c r="R6" s="35">
         <f t="shared" si="15"/>
         <v>0.67113939831370362</v>
       </c>
-      <c r="S6" s="38">
+      <c r="S6" s="35">
         <f t="shared" si="16"/>
         <v>0.6336421078461445</v>
       </c>
-      <c r="T6" s="38">
+      <c r="T6" s="35">
         <f t="shared" si="17"/>
         <v>0.63364318581884449</v>
       </c>
@@ -14867,71 +14859,71 @@
         <f t="shared" si="8"/>
         <v>8</v>
       </c>
-      <c r="C7" s="38">
+      <c r="C7" s="35">
         <f t="shared" si="0"/>
         <v>1.1929850024189648</v>
       </c>
-      <c r="D7" s="38">
+      <c r="D7" s="35">
         <f t="shared" si="1"/>
         <v>1.2353275274517228</v>
       </c>
-      <c r="E7" s="38">
+      <c r="E7" s="35">
         <f t="shared" si="2"/>
         <v>1.2008062312107133</v>
       </c>
-      <c r="F7" s="38">
+      <c r="F7" s="35">
         <f t="shared" si="3"/>
         <v>1.2377442209976384</v>
       </c>
-      <c r="G7" s="38">
+      <c r="G7" s="35">
         <f t="shared" si="4"/>
         <v>1.2637135316356372</v>
       </c>
-      <c r="H7" s="38">
+      <c r="H7" s="35">
         <f t="shared" si="5"/>
         <v>1.2211225788208682</v>
       </c>
-      <c r="I7" s="38">
+      <c r="I7" s="35">
         <f t="shared" si="6"/>
         <v>1.2746239000851547</v>
       </c>
-      <c r="J7" s="38">
+      <c r="J7" s="35">
         <f t="shared" si="7"/>
         <v>1.2714788732394366</v>
       </c>
-      <c r="L7" s="30">
+      <c r="L7" s="29">
         <f t="shared" si="9"/>
         <v>8</v>
       </c>
-      <c r="M7" s="38">
+      <c r="M7" s="35">
         <f t="shared" si="10"/>
         <v>0.8382335050083134</v>
       </c>
-      <c r="N7" s="38">
+      <c r="N7" s="35">
         <f t="shared" si="11"/>
         <v>0.80950191570881225</v>
       </c>
-      <c r="O7" s="38">
+      <c r="O7" s="35">
         <f t="shared" si="12"/>
         <v>0.83277382645803688</v>
       </c>
-      <c r="P7" s="38">
+      <c r="P7" s="35">
         <f t="shared" si="13"/>
         <v>0.80792136455623009</v>
       </c>
-      <c r="Q7" s="38">
+      <c r="Q7" s="35">
         <f t="shared" si="14"/>
         <v>0.79131858207270278</v>
       </c>
-      <c r="R7" s="38">
+      <c r="R7" s="35">
         <f t="shared" si="15"/>
         <v>0.8189186059974527</v>
       </c>
-      <c r="S7" s="38">
+      <c r="S7" s="35">
         <f t="shared" si="16"/>
         <v>0.78454515087406751</v>
       </c>
-      <c r="T7" s="38">
+      <c r="T7" s="35">
         <f t="shared" si="17"/>
         <v>0.78648573802270838</v>
       </c>
@@ -14941,71 +14933,71 @@
         <f t="shared" si="8"/>
         <v>16</v>
       </c>
-      <c r="C8" s="38">
+      <c r="C8" s="35">
         <f t="shared" si="0"/>
         <v>1.0648171374103246</v>
       </c>
-      <c r="D8" s="38">
+      <c r="D8" s="35">
         <f t="shared" si="1"/>
         <v>0.83379851143009043</v>
       </c>
-      <c r="E8" s="38">
+      <c r="E8" s="35">
         <f t="shared" si="2"/>
         <v>0.92031080592699677</v>
       </c>
-      <c r="F8" s="38">
+      <c r="F8" s="35">
         <f t="shared" si="3"/>
         <v>1.046063377981052</v>
       </c>
-      <c r="G8" s="38">
+      <c r="G8" s="35">
         <f t="shared" si="4"/>
         <v>1.0826873385012921</v>
       </c>
-      <c r="H8" s="38">
+      <c r="H8" s="35">
         <f t="shared" si="5"/>
         <v>1.0187611361492506</v>
       </c>
-      <c r="I8" s="38">
+      <c r="I8" s="35">
         <f t="shared" si="6"/>
         <v>1.0292583120204604</v>
       </c>
-      <c r="J8" s="38">
+      <c r="J8" s="35">
         <f t="shared" si="7"/>
         <v>0.9094594594594595</v>
       </c>
-      <c r="L8" s="30">
+      <c r="L8" s="29">
         <f t="shared" si="9"/>
         <v>16</v>
       </c>
-      <c r="M8" s="38">
+      <c r="M8" s="35">
         <f t="shared" si="10"/>
         <v>0.9391283863368669</v>
       </c>
-      <c r="N8" s="38">
+      <c r="N8" s="35">
         <f t="shared" si="11"/>
         <v>1.1993305172551207</v>
       </c>
-      <c r="O8" s="38">
+      <c r="O8" s="35">
         <f t="shared" si="12"/>
         <v>1.086589436481445</v>
       </c>
-      <c r="P8" s="38">
+      <c r="P8" s="35">
         <f t="shared" si="13"/>
         <v>0.95596502186133658</v>
       </c>
-      <c r="Q8" s="38">
+      <c r="Q8" s="35">
         <f t="shared" si="14"/>
         <v>0.92362768496420045</v>
       </c>
-      <c r="R8" s="38">
+      <c r="R8" s="35">
         <f t="shared" si="15"/>
         <v>0.98158436213991773</v>
       </c>
-      <c r="S8" s="38">
+      <c r="S8" s="35">
         <f t="shared" si="16"/>
         <v>0.97157340224629751</v>
       </c>
-      <c r="T8" s="38">
+      <c r="T8" s="35">
         <f t="shared" si="17"/>
         <v>1.0995542347696881</v>
       </c>
@@ -15015,71 +15007,71 @@
         <f t="shared" si="8"/>
         <v>32</v>
       </c>
-      <c r="C9" s="38">
+      <c r="C9" s="35">
         <f t="shared" si="0"/>
         <v>1.0087624349260347</v>
       </c>
-      <c r="D9" s="38">
+      <c r="D9" s="35">
         <f t="shared" si="1"/>
         <v>0.93242148834698113</v>
       </c>
-      <c r="E9" s="38">
+      <c r="E9" s="35">
         <f t="shared" si="2"/>
         <v>0.9526691683815518</v>
       </c>
-      <c r="F9" s="38">
+      <c r="F9" s="35">
         <f t="shared" si="3"/>
         <v>0.92719188550785037</v>
       </c>
-      <c r="G9" s="38">
+      <c r="G9" s="35">
         <f t="shared" si="4"/>
         <v>0.94266441821247882</v>
       </c>
-      <c r="H9" s="38">
+      <c r="H9" s="35">
         <f t="shared" si="5"/>
         <v>0.86587942821628339</v>
       </c>
-      <c r="I9" s="38">
+      <c r="I9" s="35">
         <f t="shared" si="6"/>
         <v>0.85474353154788929</v>
       </c>
-      <c r="J9" s="38">
+      <c r="J9" s="35">
         <f t="shared" si="7"/>
         <v>0.69172609330698509</v>
       </c>
-      <c r="L9" s="30">
+      <c r="L9" s="29">
         <f t="shared" si="9"/>
         <v>32</v>
       </c>
-      <c r="M9" s="38">
+      <c r="M9" s="35">
         <f t="shared" si="10"/>
         <v>0.9913136784017168</v>
       </c>
-      <c r="N9" s="38">
+      <c r="N9" s="35">
         <f t="shared" si="11"/>
         <v>1.0724763559158463</v>
       </c>
-      <c r="O9" s="38">
+      <c r="O9" s="35">
         <f t="shared" si="12"/>
         <v>1.0496823379923761</v>
       </c>
-      <c r="P9" s="38">
+      <c r="P9" s="35">
         <f t="shared" si="13"/>
         <v>1.0785254008691745</v>
       </c>
-      <c r="Q9" s="38">
+      <c r="Q9" s="35">
         <f t="shared" si="14"/>
         <v>1.0608228980322005</v>
       </c>
-      <c r="R9" s="38">
+      <c r="R9" s="35">
         <f t="shared" si="15"/>
         <v>1.1548952052828021</v>
       </c>
-      <c r="S9" s="38">
+      <c r="S9" s="35">
         <f t="shared" si="16"/>
         <v>1.1699415825809878</v>
       </c>
-      <c r="T9" s="38">
+      <c r="T9" s="35">
         <f t="shared" si="17"/>
         <v>1.4456589243572229</v>
       </c>
@@ -15089,71 +15081,71 @@
         <f t="shared" si="8"/>
         <v>64</v>
       </c>
-      <c r="C10" s="38">
+      <c r="C10" s="35">
         <f t="shared" si="0"/>
         <v>0.91525340652877163</v>
       </c>
-      <c r="D10" s="38">
+      <c r="D10" s="35">
         <f t="shared" si="1"/>
         <v>0.8761198081621574</v>
       </c>
-      <c r="E10" s="38">
+      <c r="E10" s="35">
         <f t="shared" si="2"/>
         <v>0.87770717157307732</v>
       </c>
-      <c r="F10" s="38">
+      <c r="F10" s="35">
         <f t="shared" si="3"/>
         <v>0.83776511554289335</v>
       </c>
-      <c r="G10" s="38">
+      <c r="G10" s="35">
         <f t="shared" si="4"/>
         <v>0.9425535191744957</v>
       </c>
-      <c r="H10" s="38">
+      <c r="H10" s="35">
         <f t="shared" si="5"/>
         <v>0.83068135454916359</v>
       </c>
-      <c r="I10" s="38">
+      <c r="I10" s="35">
         <f t="shared" si="6"/>
         <v>0.79136104319478406</v>
       </c>
-      <c r="J10" s="38">
+      <c r="J10" s="35">
         <f t="shared" si="7"/>
         <v>0.69221556886227553</v>
       </c>
-      <c r="L10" s="30">
+      <c r="L10" s="29">
         <f t="shared" si="9"/>
         <v>64</v>
       </c>
-      <c r="M10" s="38">
+      <c r="M10" s="35">
         <f t="shared" si="10"/>
         <v>1.092593584319606</v>
       </c>
-      <c r="N10" s="38">
+      <c r="N10" s="35">
         <f t="shared" si="11"/>
         <v>1.1413964057013013</v>
       </c>
-      <c r="O10" s="38">
+      <c r="O10" s="35">
         <f t="shared" si="12"/>
         <v>1.1393321513002366</v>
       </c>
-      <c r="P10" s="38">
+      <c r="P10" s="35">
         <f t="shared" si="13"/>
         <v>1.1936519931985641</v>
       </c>
-      <c r="Q10" s="38">
+      <c r="Q10" s="35">
         <f t="shared" si="14"/>
         <v>1.0609477124183007</v>
       </c>
-      <c r="R10" s="38">
+      <c r="R10" s="35">
         <f t="shared" si="15"/>
         <v>1.2038310412573674</v>
       </c>
-      <c r="S10" s="38">
+      <c r="S10" s="35">
         <f t="shared" si="16"/>
         <v>1.2636457260556127</v>
       </c>
-      <c r="T10" s="38">
+      <c r="T10" s="35">
         <f t="shared" si="17"/>
         <v>1.4446366782006919</v>
       </c>
@@ -15163,71 +15155,71 @@
         <f t="shared" si="8"/>
         <v>128</v>
       </c>
-      <c r="C11" s="38">
+      <c r="C11" s="35">
         <f t="shared" si="0"/>
         <v>0.8754909090909091</v>
       </c>
-      <c r="D11" s="38">
+      <c r="D11" s="35">
         <f t="shared" si="1"/>
         <v>0.89186946902654873</v>
       </c>
-      <c r="E11" s="38">
+      <c r="E11" s="35">
         <f t="shared" si="2"/>
         <v>0.86240233081711037</v>
       </c>
-      <c r="F11" s="38">
+      <c r="F11" s="35">
         <f t="shared" si="3"/>
         <v>0.8178237321516495</v>
       </c>
-      <c r="G11" s="38">
+      <c r="G11" s="35">
         <f t="shared" si="4"/>
         <v>0.86517571884984035</v>
       </c>
-      <c r="H11" s="38">
+      <c r="H11" s="35">
         <f t="shared" si="5"/>
         <v>0.81315565636518294</v>
       </c>
-      <c r="I11" s="38">
+      <c r="I11" s="35">
         <f t="shared" si="6"/>
         <v>0.75804195804195806</v>
       </c>
-      <c r="J11" s="38">
+      <c r="J11" s="35">
         <f t="shared" si="7"/>
         <v>0.67375949143563485</v>
       </c>
-      <c r="L11" s="30">
+      <c r="L11" s="29">
         <f t="shared" si="9"/>
         <v>128</v>
       </c>
-      <c r="M11" s="38">
+      <c r="M11" s="35">
         <f t="shared" si="10"/>
         <v>1.142216315002492</v>
       </c>
-      <c r="N11" s="38">
+      <c r="N11" s="35">
         <f t="shared" si="11"/>
         <v>1.1212403100775192</v>
       </c>
-      <c r="O11" s="38">
+      <c r="O11" s="35">
         <f t="shared" si="12"/>
         <v>1.159551597051597</v>
       </c>
-      <c r="P11" s="38">
+      <c r="P11" s="36">
         <f t="shared" si="13"/>
         <v>1.2227573750752558</v>
       </c>
-      <c r="Q11" s="38">
+      <c r="Q11" s="35">
         <f t="shared" si="14"/>
         <v>1.1558345642540619</v>
       </c>
-      <c r="R11" s="38">
+      <c r="R11" s="35">
         <f t="shared" si="15"/>
         <v>1.2297768479776847</v>
       </c>
-      <c r="S11" s="38">
+      <c r="S11" s="35">
         <f t="shared" si="16"/>
         <v>1.3191881918819188</v>
       </c>
-      <c r="T11" s="39">
+      <c r="T11" s="36">
         <f t="shared" si="17"/>
         <v>1.4842091469007992</v>
       </c>
@@ -15237,71 +15229,71 @@
         <f t="shared" si="8"/>
         <v>256</v>
       </c>
-      <c r="C12" s="38">
+      <c r="C12" s="35">
         <f t="shared" si="0"/>
         <v>0.86047918120493139</v>
       </c>
-      <c r="D12" s="38">
+      <c r="D12" s="35">
         <f t="shared" si="1"/>
         <v>0.88860621479193169</v>
       </c>
-      <c r="E12" s="38">
+      <c r="E12" s="35">
         <f t="shared" si="2"/>
         <v>0.85033146353901068</v>
       </c>
-      <c r="F12" s="38">
+      <c r="F12" s="35">
         <f t="shared" si="3"/>
         <v>0.86423505572441739</v>
       </c>
-      <c r="G12" s="38">
+      <c r="G12" s="35">
         <f t="shared" si="4"/>
         <v>0.83931333127126517</v>
       </c>
-      <c r="H12" s="38">
+      <c r="H12" s="35">
         <f t="shared" si="5"/>
         <v>0.83637122582440515</v>
       </c>
-      <c r="I12" s="38">
+      <c r="I12" s="35">
         <f t="shared" si="6"/>
         <v>0.78081546075889696</v>
       </c>
-      <c r="J12" s="38">
+      <c r="J12" s="35">
         <f t="shared" si="7"/>
         <v>0.6780991006877094</v>
       </c>
-      <c r="L12" s="30">
+      <c r="L12" s="29">
         <f t="shared" si="9"/>
         <v>256</v>
       </c>
-      <c r="M12" s="38">
+      <c r="M12" s="35">
         <f t="shared" si="10"/>
         <v>1.1621431660899655</v>
       </c>
-      <c r="N12" s="38">
+      <c r="N12" s="35">
         <f t="shared" si="11"/>
         <v>1.125357873210634</v>
       </c>
-      <c r="O12" s="38">
+      <c r="O12" s="35">
         <f t="shared" si="12"/>
         <v>1.1760119940029985</v>
       </c>
-      <c r="P12" s="38">
+      <c r="P12" s="35">
         <f t="shared" si="13"/>
         <v>1.157092614302462</v>
       </c>
-      <c r="Q12" s="38">
+      <c r="Q12" s="35">
         <f t="shared" si="14"/>
         <v>1.1914501566242859</v>
       </c>
-      <c r="R12" s="38">
+      <c r="R12" s="35">
         <f t="shared" si="15"/>
         <v>1.1956413242388955</v>
       </c>
-      <c r="S12" s="38">
+      <c r="S12" s="35">
         <f t="shared" si="16"/>
         <v>1.2807123453063689</v>
       </c>
-      <c r="T12" s="38">
+      <c r="T12" s="35">
         <f t="shared" si="17"/>
         <v>1.4747107008191394</v>
       </c>
@@ -15311,71 +15303,71 @@
         <f t="shared" si="8"/>
         <v>512</v>
       </c>
-      <c r="C13" s="38">
+      <c r="C13" s="35">
         <f t="shared" si="0"/>
         <v>0.92405063291139256</v>
       </c>
-      <c r="D13" s="38">
+      <c r="D13" s="35">
         <f t="shared" si="1"/>
         <v>0.97586322494133426</v>
       </c>
-      <c r="E13" s="38">
+      <c r="E13" s="35">
         <f t="shared" si="2"/>
         <v>0.93642713389369003</v>
       </c>
-      <c r="F13" s="38">
+      <c r="F13" s="35">
         <f t="shared" si="3"/>
         <v>1.0083981337480559</v>
       </c>
-      <c r="G13" s="38">
+      <c r="G13" s="35">
         <f t="shared" si="4"/>
         <v>1.0217199882594659</v>
       </c>
-      <c r="H13" s="38">
+      <c r="H13" s="35">
         <f t="shared" si="5"/>
         <v>0.95464882943143814</v>
       </c>
-      <c r="I13" s="38">
+      <c r="I13" s="35">
         <f t="shared" si="6"/>
         <v>0.89207650273224048</v>
       </c>
-      <c r="J13" s="38">
+      <c r="J13" s="35">
         <f t="shared" si="7"/>
         <v>0.7628310898827616</v>
       </c>
-      <c r="L13" s="30">
+      <c r="L13" s="29">
         <f t="shared" si="9"/>
         <v>512</v>
       </c>
-      <c r="M13" s="38">
+      <c r="M13" s="35">
         <f t="shared" si="10"/>
         <v>1.0821917808219177</v>
       </c>
-      <c r="N13" s="38">
+      <c r="N13" s="35">
         <f t="shared" si="11"/>
         <v>1.0247337684644451</v>
       </c>
-      <c r="O13" s="38">
+      <c r="O13" s="35">
         <f t="shared" si="12"/>
         <v>1.0678887484197219</v>
       </c>
-      <c r="P13" s="38">
+      <c r="P13" s="35">
         <f t="shared" si="13"/>
         <v>0.99167180752621842</v>
       </c>
-      <c r="Q13" s="38">
+      <c r="Q13" s="35">
         <f t="shared" si="14"/>
         <v>0.97874174087905763</v>
       </c>
-      <c r="R13" s="38">
+      <c r="R13" s="35">
         <f t="shared" si="15"/>
         <v>1.047505605381166</v>
       </c>
-      <c r="S13" s="38">
+      <c r="S13" s="35">
         <f t="shared" si="16"/>
         <v>1.1209800918836141</v>
       </c>
-      <c r="T13" s="38">
+      <c r="T13" s="35">
         <f t="shared" si="17"/>
         <v>1.3109061930783243</v>
       </c>
@@ -15385,71 +15377,71 @@
         <f t="shared" si="8"/>
         <v>1024</v>
       </c>
-      <c r="C14" s="38">
+      <c r="C14" s="35">
         <f t="shared" si="0"/>
         <v>1.2790811707905854</v>
       </c>
-      <c r="D14" s="38">
+      <c r="D14" s="35">
         <f t="shared" si="1"/>
         <v>1.3597809296447128</v>
       </c>
-      <c r="E14" s="38">
+      <c r="E14" s="35">
         <f t="shared" si="2"/>
         <v>1.5360233447373717</v>
       </c>
-      <c r="F14" s="38">
+      <c r="F14" s="35">
         <f t="shared" si="3"/>
         <v>1.7487666034155598</v>
       </c>
-      <c r="G14" s="38">
+      <c r="G14" s="35">
         <f t="shared" si="4"/>
         <v>1.7106668322364336</v>
       </c>
-      <c r="H14" s="38">
+      <c r="H14" s="35">
         <f t="shared" si="5"/>
         <v>1.5718976449275361</v>
       </c>
-      <c r="I14" s="38">
+      <c r="I14" s="35">
         <f t="shared" si="6"/>
         <v>1.2979189485213583</v>
       </c>
-      <c r="J14" s="38">
+      <c r="J14" s="35">
         <f t="shared" si="7"/>
         <v>1.1875</v>
       </c>
-      <c r="L14" s="30">
+      <c r="L14" s="29">
         <f t="shared" si="9"/>
         <v>1024</v>
       </c>
-      <c r="M14" s="38">
+      <c r="M14" s="35">
         <f t="shared" si="10"/>
         <v>0.78181121170121781</v>
       </c>
-      <c r="N14" s="38">
+      <c r="N14" s="35">
         <f t="shared" si="11"/>
         <v>0.73541257874625643</v>
       </c>
-      <c r="O14" s="38">
+      <c r="O14" s="35">
         <f t="shared" si="12"/>
         <v>0.65103177202751394</v>
       </c>
-      <c r="P14" s="38">
+      <c r="P14" s="35">
         <f t="shared" si="13"/>
         <v>0.57183159722222221</v>
       </c>
-      <c r="Q14" s="38">
+      <c r="Q14" s="35">
         <f t="shared" si="14"/>
         <v>0.58456736353077821</v>
       </c>
-      <c r="R14" s="38">
+      <c r="R14" s="35">
         <f t="shared" si="15"/>
         <v>0.63617373766476992</v>
       </c>
-      <c r="S14" s="38">
+      <c r="S14" s="35">
         <f t="shared" si="16"/>
         <v>0.77046413502109701</v>
       </c>
-      <c r="T14" s="38">
+      <c r="T14" s="35">
         <f t="shared" si="17"/>
         <v>0.84210526315789469</v>
       </c>
@@ -15459,89 +15451,89 @@
         <f t="shared" si="8"/>
         <v>2048</v>
       </c>
-      <c r="C15" s="38">
+      <c r="C15" s="35">
         <f t="shared" si="0"/>
         <v>2.224679735765291</v>
       </c>
-      <c r="D15" s="38">
+      <c r="D15" s="35">
         <f t="shared" si="1"/>
         <v>2.7255841548010227</v>
       </c>
-      <c r="E15" s="38">
+      <c r="E15" s="35">
         <f t="shared" si="2"/>
         <v>3.0606265772142551</v>
       </c>
-      <c r="F15" s="38">
+      <c r="F15" s="36">
         <f t="shared" si="3"/>
         <v>3.5879996977253836</v>
       </c>
-      <c r="G15" s="39">
+      <c r="G15" s="36">
         <f t="shared" si="4"/>
         <v>3.8726644685193907</v>
       </c>
-      <c r="H15" s="38">
+      <c r="H15" s="35">
         <f t="shared" si="5"/>
         <v>3.5434412265758093</v>
       </c>
-      <c r="I15" s="38">
+      <c r="I15" s="35">
         <f t="shared" si="6"/>
         <v>3.3803819322105566</v>
       </c>
-      <c r="J15" s="38">
+      <c r="J15" s="35">
         <f t="shared" si="7"/>
         <v>2.5675852627819773</v>
       </c>
-      <c r="L15" s="30">
+      <c r="L15" s="29">
         <f t="shared" si="9"/>
         <v>2048</v>
       </c>
-      <c r="M15" s="38">
+      <c r="M15" s="35">
         <f t="shared" si="10"/>
         <v>0.44950290323744035</v>
       </c>
-      <c r="N15" s="38">
+      <c r="N15" s="35">
         <f t="shared" si="11"/>
         <v>0.36689382649900371</v>
       </c>
-      <c r="O15" s="38">
+      <c r="O15" s="35">
         <f t="shared" si="12"/>
         <v>0.32673048304709806</v>
       </c>
-      <c r="P15" s="38">
+      <c r="P15" s="35">
         <f t="shared" si="13"/>
         <v>0.27870682392586349</v>
       </c>
-      <c r="Q15" s="38">
+      <c r="Q15" s="35">
         <f t="shared" si="14"/>
         <v>0.25822015001013582</v>
       </c>
-      <c r="R15" s="38">
+      <c r="R15" s="35">
         <f t="shared" si="15"/>
         <v>0.28221153846153846</v>
       </c>
-      <c r="S15" s="38">
+      <c r="S15" s="35">
         <f t="shared" si="16"/>
         <v>0.29582456067207269</v>
       </c>
-      <c r="T15" s="38">
+      <c r="T15" s="35">
         <f t="shared" si="17"/>
         <v>0.38947100004636281</v>
       </c>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="B18" s="21" t="s">
+      <c r="B18" s="20" t="s">
         <v>12</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="L18" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="L18" s="20" t="s">
         <v>13</v>
       </c>
       <c r="M18"/>
-      <c r="N18" s="26"/>
+      <c r="N18" s="25"/>
       <c r="O18" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P18" s="3"/>
       <c r="Q18" s="3"/>
@@ -15549,100 +15541,100 @@
       <c r="S18" s="3"/>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="B19" s="31" t="s">
+      <c r="B19" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C19" s="32" t="s">
+      <c r="C19" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="D19" s="33" t="s">
+      <c r="D19" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="E19" s="34" t="s">
+      <c r="E19" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="F19" s="34" t="s">
+      <c r="F19" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="G19" s="34" t="s">
+      <c r="G19" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="H19" s="34" t="s">
+      <c r="H19" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="I19" s="34" t="s">
+      <c r="I19" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="L19" s="31" t="s">
+      <c r="L19" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="M19" s="32" t="s">
+      <c r="M19" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="N19" s="35" t="s">
+      <c r="N19" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="O19" s="34" t="s">
+      <c r="O19" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="P19" s="34" t="s">
+      <c r="P19" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="Q19" s="34" t="s">
+      <c r="Q19" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="R19" s="34" t="s">
+      <c r="R19" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="S19" s="34" t="s">
+      <c r="S19" s="33" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="B20" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="23"/>
+      <c r="B20" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="22"/>
       <c r="D20" s="5">
         <f>AVERAGE(E20:I20)</f>
         <v>12455</v>
       </c>
-      <c r="E20" s="24">
+      <c r="E20" s="23">
         <v>12759</v>
       </c>
-      <c r="F20" s="24">
+      <c r="F20" s="23">
         <v>12310</v>
       </c>
-      <c r="G20" s="24">
+      <c r="G20" s="23">
         <v>12342</v>
       </c>
-      <c r="H20" s="24">
+      <c r="H20" s="23">
         <v>12228</v>
       </c>
-      <c r="I20" s="24">
+      <c r="I20" s="23">
         <v>12636</v>
       </c>
-      <c r="L20" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="M20" s="23"/>
-      <c r="N20" s="27">
+      <c r="L20" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="M20" s="22"/>
+      <c r="N20" s="26">
         <f>AVERAGE(O20:S20)</f>
         <v>5993.2</v>
       </c>
-      <c r="O20" s="24">
+      <c r="O20" s="23">
         <v>5915</v>
       </c>
-      <c r="P20" s="24">
+      <c r="P20" s="23">
         <v>6023</v>
       </c>
-      <c r="Q20" s="24">
+      <c r="Q20" s="23">
         <v>5937</v>
       </c>
-      <c r="R20" s="24">
+      <c r="R20" s="23">
         <v>6109</v>
       </c>
-      <c r="S20" s="24">
+      <c r="S20" s="23">
         <v>5982</v>
       </c>
     </row>
@@ -15678,23 +15670,23 @@
       <c r="M21" s="6">
         <v>1</v>
       </c>
-      <c r="N21" s="27">
+      <c r="N21" s="26">
         <f t="shared" ref="N21:N84" si="18">AVERAGE(O21:S21)</f>
         <v>6022.8</v>
       </c>
-      <c r="O21" s="24">
+      <c r="O21" s="23">
         <v>6004</v>
       </c>
-      <c r="P21" s="24">
+      <c r="P21" s="23">
         <v>6009</v>
       </c>
-      <c r="Q21" s="24">
+      <c r="Q21" s="23">
         <v>6108</v>
       </c>
-      <c r="R21" s="24">
+      <c r="R21" s="23">
         <v>6079</v>
       </c>
-      <c r="S21" s="24">
+      <c r="S21" s="23">
         <v>5914</v>
       </c>
     </row>
@@ -15732,23 +15724,23 @@
         <f t="shared" ref="M22:M32" si="21">M21*2</f>
         <v>2</v>
       </c>
-      <c r="N22" s="27">
+      <c r="N22" s="26">
         <f t="shared" si="18"/>
         <v>5628.8</v>
       </c>
-      <c r="O22" s="24">
+      <c r="O22" s="23">
         <v>5700</v>
       </c>
-      <c r="P22" s="24">
+      <c r="P22" s="23">
         <v>5674</v>
       </c>
-      <c r="Q22" s="24">
+      <c r="Q22" s="23">
         <v>5422</v>
       </c>
-      <c r="R22" s="24">
+      <c r="R22" s="23">
         <v>5657</v>
       </c>
-      <c r="S22" s="24">
+      <c r="S22" s="23">
         <v>5691</v>
       </c>
     </row>
@@ -15786,23 +15778,23 @@
         <f t="shared" si="21"/>
         <v>4</v>
       </c>
-      <c r="N23" s="27">
+      <c r="N23" s="26">
         <f t="shared" si="18"/>
         <v>4675</v>
       </c>
-      <c r="O23" s="24">
+      <c r="O23" s="23">
         <v>4750</v>
       </c>
-      <c r="P23" s="24">
+      <c r="P23" s="23">
         <v>4597</v>
       </c>
-      <c r="Q23" s="24">
+      <c r="Q23" s="23">
         <v>4737</v>
       </c>
-      <c r="R23" s="24">
+      <c r="R23" s="23">
         <v>4610</v>
       </c>
-      <c r="S23" s="24">
+      <c r="S23" s="23">
         <v>4681</v>
       </c>
     </row>
@@ -15840,23 +15832,23 @@
         <f t="shared" si="21"/>
         <v>8</v>
       </c>
-      <c r="N24" s="27">
+      <c r="N24" s="26">
         <f t="shared" si="18"/>
         <v>4134</v>
       </c>
-      <c r="O24" s="24">
+      <c r="O24" s="23">
         <v>4159</v>
       </c>
-      <c r="P24" s="24">
+      <c r="P24" s="23">
         <v>4181</v>
       </c>
-      <c r="Q24" s="24">
+      <c r="Q24" s="23">
         <v>4112</v>
       </c>
-      <c r="R24" s="24">
+      <c r="R24" s="23">
         <v>4160</v>
       </c>
-      <c r="S24" s="24">
+      <c r="S24" s="23">
         <v>4058</v>
       </c>
     </row>
@@ -15894,23 +15886,23 @@
         <f t="shared" si="21"/>
         <v>16</v>
       </c>
-      <c r="N25" s="27">
+      <c r="N25" s="26">
         <f t="shared" si="18"/>
         <v>3986.6</v>
       </c>
-      <c r="O25" s="24">
+      <c r="O25" s="23">
         <v>4012</v>
       </c>
-      <c r="P25" s="24">
+      <c r="P25" s="23">
         <v>3994</v>
       </c>
-      <c r="Q25" s="24">
+      <c r="Q25" s="23">
         <v>4016</v>
       </c>
-      <c r="R25" s="24">
+      <c r="R25" s="23">
         <v>3885</v>
       </c>
-      <c r="S25" s="24">
+      <c r="S25" s="23">
         <v>4026</v>
       </c>
     </row>
@@ -15948,23 +15940,23 @@
         <f t="shared" si="21"/>
         <v>32</v>
       </c>
-      <c r="N26" s="27">
+      <c r="N26" s="26">
         <f t="shared" si="18"/>
         <v>3880.2</v>
       </c>
-      <c r="O26" s="24">
+      <c r="O26" s="23">
         <v>3980</v>
       </c>
-      <c r="P26" s="24">
+      <c r="P26" s="23">
         <v>3812</v>
       </c>
-      <c r="Q26" s="24">
+      <c r="Q26" s="23">
         <v>3793</v>
       </c>
-      <c r="R26" s="24">
+      <c r="R26" s="23">
         <v>3880</v>
       </c>
-      <c r="S26" s="24">
+      <c r="S26" s="23">
         <v>3936</v>
       </c>
     </row>
@@ -16002,23 +15994,23 @@
         <f t="shared" si="21"/>
         <v>64</v>
       </c>
-      <c r="N27" s="27">
+      <c r="N27" s="26">
         <f t="shared" si="18"/>
         <v>4080.4</v>
       </c>
-      <c r="O27" s="24">
+      <c r="O27" s="23">
         <v>4124</v>
       </c>
-      <c r="P27" s="24">
+      <c r="P27" s="23">
         <v>4171</v>
       </c>
-      <c r="Q27" s="24">
+      <c r="Q27" s="23">
         <v>4040</v>
       </c>
-      <c r="R27" s="24">
+      <c r="R27" s="23">
         <v>4063</v>
       </c>
-      <c r="S27" s="24">
+      <c r="S27" s="23">
         <v>4004</v>
       </c>
     </row>
@@ -16056,23 +16048,23 @@
         <f t="shared" si="21"/>
         <v>128</v>
       </c>
-      <c r="N28" s="27">
+      <c r="N28" s="26">
         <f t="shared" si="18"/>
         <v>4125</v>
       </c>
-      <c r="O28" s="24">
+      <c r="O28" s="23">
         <v>4122</v>
       </c>
-      <c r="P28" s="24">
+      <c r="P28" s="23">
         <v>4172</v>
       </c>
-      <c r="Q28" s="24">
+      <c r="Q28" s="23">
         <v>4150</v>
       </c>
-      <c r="R28" s="24">
+      <c r="R28" s="23">
         <v>4026</v>
       </c>
-      <c r="S28" s="24">
+      <c r="S28" s="23">
         <v>4155</v>
       </c>
     </row>
@@ -16110,23 +16102,23 @@
         <f t="shared" si="21"/>
         <v>256</v>
       </c>
-      <c r="N29" s="27">
+      <c r="N29" s="26">
         <f t="shared" si="18"/>
         <v>4299</v>
       </c>
-      <c r="O29" s="24">
+      <c r="O29" s="23">
         <v>4239</v>
       </c>
-      <c r="P29" s="24">
+      <c r="P29" s="23">
         <v>4358</v>
       </c>
-      <c r="Q29" s="24">
+      <c r="Q29" s="23">
         <v>4363</v>
       </c>
-      <c r="R29" s="24">
+      <c r="R29" s="23">
         <v>4199</v>
       </c>
-      <c r="S29" s="24">
+      <c r="S29" s="23">
         <v>4336</v>
       </c>
     </row>
@@ -16164,23 +16156,23 @@
         <f t="shared" si="21"/>
         <v>512</v>
       </c>
-      <c r="N30" s="27">
+      <c r="N30" s="26">
         <f t="shared" si="18"/>
         <v>4550.3999999999996</v>
       </c>
-      <c r="O30" s="24">
+      <c r="O30" s="23">
         <v>4621</v>
       </c>
-      <c r="P30" s="24">
+      <c r="P30" s="23">
         <v>4526</v>
       </c>
-      <c r="Q30" s="24">
+      <c r="Q30" s="23">
         <v>4605</v>
       </c>
-      <c r="R30" s="24">
+      <c r="R30" s="23">
         <v>4494</v>
       </c>
-      <c r="S30" s="24">
+      <c r="S30" s="23">
         <v>4506</v>
       </c>
     </row>
@@ -16218,23 +16210,23 @@
         <f t="shared" si="21"/>
         <v>1024</v>
       </c>
-      <c r="N31" s="27">
+      <c r="N31" s="26">
         <f t="shared" si="18"/>
         <v>5302.4</v>
       </c>
-      <c r="O31" s="24">
+      <c r="O31" s="23">
         <v>5290</v>
       </c>
-      <c r="P31" s="24">
+      <c r="P31" s="23">
         <v>5323</v>
       </c>
-      <c r="Q31" s="24">
+      <c r="Q31" s="23">
         <v>5261</v>
       </c>
-      <c r="R31" s="24">
+      <c r="R31" s="23">
         <v>5289</v>
       </c>
-      <c r="S31" s="24">
+      <c r="S31" s="23">
         <v>5349</v>
       </c>
     </row>
@@ -16272,23 +16264,23 @@
         <f t="shared" si="21"/>
         <v>2048</v>
       </c>
-      <c r="N32" s="27">
+      <c r="N32" s="26">
         <f t="shared" si="18"/>
         <v>7478.2</v>
       </c>
-      <c r="O32" s="24">
+      <c r="O32" s="23">
         <v>7288</v>
       </c>
-      <c r="P32" s="24">
+      <c r="P32" s="23">
         <v>7507</v>
       </c>
-      <c r="Q32" s="24">
+      <c r="Q32" s="23">
         <v>7629</v>
       </c>
-      <c r="R32" s="24">
+      <c r="R32" s="23">
         <v>7442</v>
       </c>
-      <c r="S32" s="24">
+      <c r="S32" s="23">
         <v>7525</v>
       </c>
     </row>
@@ -16324,23 +16316,23 @@
       <c r="M33" s="6">
         <v>1</v>
       </c>
-      <c r="N33" s="27">
+      <c r="N33" s="26">
         <f t="shared" si="18"/>
         <v>6121.2</v>
       </c>
-      <c r="O33" s="24">
+      <c r="O33" s="23">
         <v>6106</v>
       </c>
-      <c r="P33" s="24">
+      <c r="P33" s="23">
         <v>6119</v>
       </c>
-      <c r="Q33" s="24">
+      <c r="Q33" s="23">
         <v>6117</v>
       </c>
-      <c r="R33" s="24">
+      <c r="R33" s="23">
         <v>6119</v>
       </c>
-      <c r="S33" s="24">
+      <c r="S33" s="23">
         <v>6145</v>
       </c>
     </row>
@@ -16378,23 +16370,23 @@
         <f t="shared" ref="M34:M44" si="23">M33*2</f>
         <v>2</v>
       </c>
-      <c r="N34" s="27">
+      <c r="N34" s="26">
         <f t="shared" si="18"/>
         <v>5525.2</v>
       </c>
-      <c r="O34" s="24">
+      <c r="O34" s="23">
         <v>5493</v>
       </c>
-      <c r="P34" s="24">
+      <c r="P34" s="23">
         <v>5537</v>
       </c>
-      <c r="Q34" s="24">
+      <c r="Q34" s="23">
         <v>5552</v>
       </c>
-      <c r="R34" s="24">
+      <c r="R34" s="23">
         <v>5605</v>
       </c>
-      <c r="S34" s="24">
+      <c r="S34" s="23">
         <v>5439</v>
       </c>
     </row>
@@ -16432,23 +16424,23 @@
         <f t="shared" si="23"/>
         <v>4</v>
       </c>
-      <c r="N35" s="27">
+      <c r="N35" s="26">
         <f t="shared" si="18"/>
         <v>4249</v>
       </c>
-      <c r="O35" s="24">
+      <c r="O35" s="23">
         <v>4152</v>
       </c>
-      <c r="P35" s="24">
+      <c r="P35" s="23">
         <v>4163</v>
       </c>
-      <c r="Q35" s="24">
+      <c r="Q35" s="23">
         <v>4305</v>
       </c>
-      <c r="R35" s="24">
+      <c r="R35" s="23">
         <v>4331</v>
       </c>
-      <c r="S35" s="24">
+      <c r="S35" s="23">
         <v>4294</v>
       </c>
     </row>
@@ -16486,23 +16478,23 @@
         <f t="shared" si="23"/>
         <v>8</v>
       </c>
-      <c r="N36" s="27">
+      <c r="N36" s="26">
         <f t="shared" si="18"/>
         <v>3169.2</v>
       </c>
-      <c r="O36" s="24">
+      <c r="O36" s="23">
         <v>3173</v>
       </c>
-      <c r="P36" s="24">
+      <c r="P36" s="23">
         <v>3105</v>
       </c>
-      <c r="Q36" s="24">
+      <c r="Q36" s="23">
         <v>3187</v>
       </c>
-      <c r="R36" s="24">
+      <c r="R36" s="23">
         <v>3163</v>
       </c>
-      <c r="S36" s="24">
+      <c r="S36" s="23">
         <v>3218</v>
       </c>
     </row>
@@ -16540,23 +16532,23 @@
         <f t="shared" si="23"/>
         <v>16</v>
       </c>
-      <c r="N37" s="27">
+      <c r="N37" s="26">
         <f t="shared" si="18"/>
         <v>3009.6</v>
       </c>
-      <c r="O37" s="24">
+      <c r="O37" s="23">
         <v>2511</v>
       </c>
-      <c r="P37" s="24">
+      <c r="P37" s="23">
         <v>3492</v>
       </c>
-      <c r="Q37" s="24">
+      <c r="Q37" s="23">
         <v>3427</v>
       </c>
-      <c r="R37" s="24">
+      <c r="R37" s="23">
         <v>3067</v>
       </c>
-      <c r="S37" s="24">
+      <c r="S37" s="23">
         <v>2551</v>
       </c>
     </row>
@@ -16594,23 +16586,23 @@
         <f t="shared" si="23"/>
         <v>32</v>
       </c>
-      <c r="N38" s="27">
+      <c r="N38" s="26">
         <f t="shared" si="18"/>
         <v>2222.6</v>
       </c>
-      <c r="O38" s="24">
+      <c r="O38" s="23">
         <v>2236</v>
       </c>
-      <c r="P38" s="24">
+      <c r="P38" s="23">
         <v>2206</v>
       </c>
-      <c r="Q38" s="24">
+      <c r="Q38" s="23">
         <v>2299</v>
       </c>
-      <c r="R38" s="24">
+      <c r="R38" s="23">
         <v>2164</v>
       </c>
-      <c r="S38" s="24">
+      <c r="S38" s="23">
         <v>2208</v>
       </c>
     </row>
@@ -16648,23 +16640,23 @@
         <f t="shared" si="23"/>
         <v>64</v>
       </c>
-      <c r="N39" s="27">
+      <c r="N39" s="26">
         <f t="shared" si="18"/>
         <v>2210.1999999999998</v>
       </c>
-      <c r="O39" s="24">
+      <c r="O39" s="23">
         <v>2112</v>
       </c>
-      <c r="P39" s="24">
+      <c r="P39" s="23">
         <v>2425</v>
       </c>
-      <c r="Q39" s="24">
+      <c r="Q39" s="23">
         <v>2186</v>
       </c>
-      <c r="R39" s="24">
+      <c r="R39" s="23">
         <v>2188</v>
       </c>
-      <c r="S39" s="24">
+      <c r="S39" s="23">
         <v>2140</v>
       </c>
     </row>
@@ -16702,23 +16694,23 @@
         <f t="shared" si="23"/>
         <v>128</v>
       </c>
-      <c r="N40" s="27">
+      <c r="N40" s="26">
         <f t="shared" si="18"/>
         <v>2169.6</v>
       </c>
-      <c r="O40" s="24">
+      <c r="O40" s="23">
         <v>2204</v>
       </c>
-      <c r="P40" s="24">
+      <c r="P40" s="23">
         <v>2103</v>
       </c>
-      <c r="Q40" s="24">
+      <c r="Q40" s="23">
         <v>2203</v>
       </c>
-      <c r="R40" s="24">
+      <c r="R40" s="23">
         <v>2170</v>
       </c>
-      <c r="S40" s="24">
+      <c r="S40" s="23">
         <v>2168</v>
       </c>
     </row>
@@ -16756,23 +16748,23 @@
         <f t="shared" si="23"/>
         <v>256</v>
       </c>
-      <c r="N41" s="27">
+      <c r="N41" s="26">
         <f t="shared" si="18"/>
         <v>2201.1999999999998</v>
       </c>
-      <c r="O41" s="24">
+      <c r="O41" s="23">
         <v>2236</v>
       </c>
-      <c r="P41" s="24">
+      <c r="P41" s="23">
         <v>2306</v>
       </c>
-      <c r="Q41" s="24">
+      <c r="Q41" s="23">
         <v>2157</v>
       </c>
-      <c r="R41" s="24">
+      <c r="R41" s="23">
         <v>2137</v>
       </c>
-      <c r="S41" s="24">
+      <c r="S41" s="23">
         <v>2170</v>
       </c>
     </row>
@@ -16810,23 +16802,23 @@
         <f t="shared" si="23"/>
         <v>512</v>
       </c>
-      <c r="N42" s="27">
+      <c r="N42" s="26">
         <f t="shared" si="18"/>
         <v>2386.4</v>
       </c>
-      <c r="O42" s="24">
+      <c r="O42" s="23">
         <v>2315</v>
       </c>
-      <c r="P42" s="24">
+      <c r="P42" s="23">
         <v>2530</v>
       </c>
-      <c r="Q42" s="24">
+      <c r="Q42" s="23">
         <v>2387</v>
       </c>
-      <c r="R42" s="24">
+      <c r="R42" s="23">
         <v>2372</v>
       </c>
-      <c r="S42" s="24">
+      <c r="S42" s="23">
         <v>2328</v>
       </c>
     </row>
@@ -16864,23 +16856,23 @@
         <f t="shared" si="23"/>
         <v>1024</v>
       </c>
-      <c r="N43" s="27">
+      <c r="N43" s="26">
         <f t="shared" si="18"/>
         <v>2848.4</v>
       </c>
-      <c r="O43" s="24">
+      <c r="O43" s="23">
         <v>2890</v>
       </c>
-      <c r="P43" s="24">
+      <c r="P43" s="23">
         <v>2859</v>
       </c>
-      <c r="Q43" s="24">
+      <c r="Q43" s="23">
         <v>2761</v>
       </c>
-      <c r="R43" s="24">
+      <c r="R43" s="23">
         <v>2893</v>
       </c>
-      <c r="S43" s="24">
+      <c r="S43" s="23">
         <v>2839</v>
       </c>
     </row>
@@ -16918,23 +16910,23 @@
         <f t="shared" si="23"/>
         <v>2048</v>
       </c>
-      <c r="N44" s="27">
+      <c r="N44" s="26">
         <f t="shared" si="18"/>
         <v>4382.3999999999996</v>
       </c>
-      <c r="O44" s="24">
+      <c r="O44" s="23">
         <v>4399</v>
       </c>
-      <c r="P44" s="24">
+      <c r="P44" s="23">
         <v>4452</v>
       </c>
-      <c r="Q44" s="24">
+      <c r="Q44" s="23">
         <v>4388</v>
       </c>
-      <c r="R44" s="24">
+      <c r="R44" s="23">
         <v>4426</v>
       </c>
-      <c r="S44" s="24">
+      <c r="S44" s="23">
         <v>4247</v>
       </c>
     </row>
@@ -16970,23 +16962,23 @@
       <c r="M45" s="6">
         <v>1</v>
       </c>
-      <c r="N45" s="27">
+      <c r="N45" s="26">
         <f t="shared" si="18"/>
         <v>5977.6</v>
       </c>
-      <c r="O45" s="24">
+      <c r="O45" s="23">
         <v>5970</v>
       </c>
-      <c r="P45" s="24">
+      <c r="P45" s="23">
         <v>5918</v>
       </c>
-      <c r="Q45" s="24">
+      <c r="Q45" s="23">
         <v>6037</v>
       </c>
-      <c r="R45" s="24">
+      <c r="R45" s="23">
         <v>6007</v>
       </c>
-      <c r="S45" s="24">
+      <c r="S45" s="23">
         <v>5956</v>
       </c>
     </row>
@@ -17024,23 +17016,23 @@
         <f t="shared" ref="M46:M56" si="25">M45*2</f>
         <v>2</v>
       </c>
-      <c r="N46" s="27">
+      <c r="N46" s="26">
         <f t="shared" si="18"/>
         <v>5487.2</v>
       </c>
-      <c r="O46" s="24">
+      <c r="O46" s="23">
         <v>5446</v>
       </c>
-      <c r="P46" s="24">
+      <c r="P46" s="23">
         <v>5393</v>
       </c>
-      <c r="Q46" s="24">
+      <c r="Q46" s="23">
         <v>5505</v>
       </c>
-      <c r="R46" s="24">
+      <c r="R46" s="23">
         <v>5551</v>
       </c>
-      <c r="S46" s="24">
+      <c r="S46" s="23">
         <v>5541</v>
       </c>
     </row>
@@ -17078,23 +17070,23 @@
         <f t="shared" si="25"/>
         <v>4</v>
       </c>
-      <c r="N47" s="27">
+      <c r="N47" s="26">
         <f t="shared" si="18"/>
         <v>4189.3999999999996</v>
       </c>
-      <c r="O47" s="24">
+      <c r="O47" s="23">
         <v>4173</v>
       </c>
-      <c r="P47" s="24">
+      <c r="P47" s="23">
         <v>4121</v>
       </c>
-      <c r="Q47" s="24">
+      <c r="Q47" s="23">
         <v>4266</v>
       </c>
-      <c r="R47" s="24">
+      <c r="R47" s="23">
         <v>4167</v>
       </c>
-      <c r="S47" s="24">
+      <c r="S47" s="23">
         <v>4220</v>
       </c>
     </row>
@@ -17132,23 +17124,23 @@
         <f t="shared" si="25"/>
         <v>8</v>
       </c>
-      <c r="N48" s="27">
+      <c r="N48" s="26">
         <f t="shared" si="18"/>
         <v>2927.2</v>
       </c>
-      <c r="O48" s="24">
+      <c r="O48" s="23">
         <v>2957</v>
       </c>
-      <c r="P48" s="24">
+      <c r="P48" s="23">
         <v>2848</v>
       </c>
-      <c r="Q48" s="24">
+      <c r="Q48" s="23">
         <v>2888</v>
       </c>
-      <c r="R48" s="24">
+      <c r="R48" s="23">
         <v>3058</v>
       </c>
-      <c r="S48" s="24">
+      <c r="S48" s="23">
         <v>2885</v>
       </c>
     </row>
@@ -17186,23 +17178,23 @@
         <f t="shared" si="25"/>
         <v>16</v>
       </c>
-      <c r="N49" s="27">
+      <c r="N49" s="26">
         <f t="shared" si="18"/>
         <v>2213.6</v>
       </c>
-      <c r="O49" s="24">
+      <c r="O49" s="23">
         <v>2027</v>
       </c>
-      <c r="P49" s="24">
+      <c r="P49" s="23">
         <v>2007</v>
       </c>
-      <c r="Q49" s="24">
+      <c r="Q49" s="23">
         <v>2040</v>
       </c>
-      <c r="R49" s="24">
+      <c r="R49" s="23">
         <v>2963</v>
       </c>
-      <c r="S49" s="24">
+      <c r="S49" s="23">
         <v>2031</v>
       </c>
     </row>
@@ -17240,23 +17232,23 @@
         <f t="shared" si="25"/>
         <v>32</v>
       </c>
-      <c r="N50" s="27">
+      <c r="N50" s="26">
         <f t="shared" si="18"/>
         <v>1652.2</v>
       </c>
-      <c r="O50" s="24">
+      <c r="O50" s="23">
         <v>1641</v>
       </c>
-      <c r="P50" s="24">
+      <c r="P50" s="23">
         <v>1615</v>
       </c>
-      <c r="Q50" s="24">
+      <c r="Q50" s="23">
         <v>1686</v>
       </c>
-      <c r="R50" s="24">
+      <c r="R50" s="23">
         <v>1628</v>
       </c>
-      <c r="S50" s="24">
+      <c r="S50" s="23">
         <v>1691</v>
       </c>
     </row>
@@ -17294,23 +17286,23 @@
         <f t="shared" si="25"/>
         <v>64</v>
       </c>
-      <c r="N51" s="27">
+      <c r="N51" s="26">
         <f t="shared" si="18"/>
         <v>1542.2</v>
       </c>
-      <c r="O51" s="24">
+      <c r="O51" s="23">
         <v>1546</v>
       </c>
-      <c r="P51" s="24">
+      <c r="P51" s="23">
         <v>1574</v>
       </c>
-      <c r="Q51" s="24">
+      <c r="Q51" s="23">
         <v>1557</v>
       </c>
-      <c r="R51" s="24">
+      <c r="R51" s="23">
         <v>1507</v>
       </c>
-      <c r="S51" s="24">
+      <c r="S51" s="23">
         <v>1527</v>
       </c>
     </row>
@@ -17348,23 +17340,23 @@
         <f t="shared" si="25"/>
         <v>128</v>
       </c>
-      <c r="N52" s="27">
+      <c r="N52" s="26">
         <f t="shared" si="18"/>
         <v>1510.2</v>
       </c>
-      <c r="O52" s="24">
+      <c r="O52" s="23">
         <v>1477</v>
       </c>
-      <c r="P52" s="24">
+      <c r="P52" s="23">
         <v>1524</v>
       </c>
-      <c r="Q52" s="24">
+      <c r="Q52" s="23">
         <v>1485</v>
       </c>
-      <c r="R52" s="24">
+      <c r="R52" s="23">
         <v>1571</v>
       </c>
-      <c r="S52" s="24">
+      <c r="S52" s="23">
         <v>1494</v>
       </c>
     </row>
@@ -17402,23 +17394,23 @@
         <f t="shared" si="25"/>
         <v>256</v>
       </c>
-      <c r="N53" s="27">
+      <c r="N53" s="26">
         <f t="shared" si="18"/>
         <v>1568.8</v>
       </c>
-      <c r="O53" s="24">
+      <c r="O53" s="23">
         <v>1520</v>
       </c>
-      <c r="P53" s="24">
+      <c r="P53" s="23">
         <v>1593</v>
       </c>
-      <c r="Q53" s="24">
+      <c r="Q53" s="23">
         <v>1653</v>
       </c>
-      <c r="R53" s="24">
+      <c r="R53" s="23">
         <v>1529</v>
       </c>
-      <c r="S53" s="24">
+      <c r="S53" s="23">
         <v>1549</v>
       </c>
     </row>
@@ -17456,23 +17448,23 @@
         <f t="shared" si="25"/>
         <v>512</v>
       </c>
-      <c r="N54" s="27">
+      <c r="N54" s="26">
         <f t="shared" si="18"/>
         <v>1689.4</v>
       </c>
-      <c r="O54" s="24">
+      <c r="O54" s="23">
         <v>1665</v>
       </c>
-      <c r="P54" s="24">
+      <c r="P54" s="23">
         <v>1641</v>
       </c>
-      <c r="Q54" s="24">
+      <c r="Q54" s="23">
         <v>1778</v>
       </c>
-      <c r="R54" s="24">
+      <c r="R54" s="23">
         <v>1648</v>
       </c>
-      <c r="S54" s="24">
+      <c r="S54" s="23">
         <v>1715</v>
       </c>
     </row>
@@ -17510,23 +17502,23 @@
         <f t="shared" si="25"/>
         <v>1024</v>
       </c>
-      <c r="N55" s="27">
+      <c r="N55" s="26">
         <f t="shared" si="18"/>
         <v>1987.6</v>
       </c>
-      <c r="O55" s="24">
+      <c r="O55" s="23">
         <v>1971</v>
       </c>
-      <c r="P55" s="24">
+      <c r="P55" s="23">
         <v>1997</v>
       </c>
-      <c r="Q55" s="24">
+      <c r="Q55" s="23">
         <v>2009</v>
       </c>
-      <c r="R55" s="24">
+      <c r="R55" s="23">
         <v>1980</v>
       </c>
-      <c r="S55" s="24">
+      <c r="S55" s="23">
         <v>1981</v>
       </c>
     </row>
@@ -17564,23 +17556,23 @@
         <f t="shared" si="25"/>
         <v>2048</v>
       </c>
-      <c r="N56" s="27">
+      <c r="N56" s="26">
         <f t="shared" si="18"/>
         <v>3249.4</v>
       </c>
-      <c r="O56" s="24">
+      <c r="O56" s="23">
         <v>3163</v>
       </c>
-      <c r="P56" s="24">
+      <c r="P56" s="23">
         <v>3311</v>
       </c>
-      <c r="Q56" s="24">
+      <c r="Q56" s="23">
         <v>3174</v>
       </c>
-      <c r="R56" s="24">
+      <c r="R56" s="23">
         <v>3272</v>
       </c>
-      <c r="S56" s="24">
+      <c r="S56" s="23">
         <v>3327</v>
       </c>
     </row>
@@ -17616,23 +17608,23 @@
       <c r="M57" s="6">
         <v>1</v>
       </c>
-      <c r="N57" s="27">
+      <c r="N57" s="26">
         <f t="shared" si="18"/>
         <v>6028.4</v>
       </c>
-      <c r="O57" s="24">
+      <c r="O57" s="23">
         <v>6059</v>
       </c>
-      <c r="P57" s="24">
+      <c r="P57" s="23">
         <v>6067</v>
       </c>
-      <c r="Q57" s="24">
+      <c r="Q57" s="23">
         <v>5840</v>
       </c>
-      <c r="R57" s="24">
+      <c r="R57" s="23">
         <v>6038</v>
       </c>
-      <c r="S57" s="24">
+      <c r="S57" s="23">
         <v>6138</v>
       </c>
     </row>
@@ -17670,23 +17662,23 @@
         <f t="shared" ref="M58:M68" si="27">M57*2</f>
         <v>2</v>
       </c>
-      <c r="N58" s="27">
+      <c r="N58" s="26">
         <f t="shared" si="18"/>
         <v>5436.6</v>
       </c>
-      <c r="O58" s="24">
+      <c r="O58" s="23">
         <v>5474</v>
       </c>
-      <c r="P58" s="24">
+      <c r="P58" s="23">
         <v>5434</v>
       </c>
-      <c r="Q58" s="24">
+      <c r="Q58" s="23">
         <v>5374</v>
       </c>
-      <c r="R58" s="24">
+      <c r="R58" s="23">
         <v>5550</v>
       </c>
-      <c r="S58" s="24">
+      <c r="S58" s="23">
         <v>5351</v>
       </c>
     </row>
@@ -17724,23 +17716,23 @@
         <f t="shared" si="27"/>
         <v>4</v>
       </c>
-      <c r="N59" s="27">
+      <c r="N59" s="26">
         <f t="shared" si="18"/>
         <v>4077.4</v>
       </c>
-      <c r="O59" s="24">
+      <c r="O59" s="23">
         <v>4153</v>
       </c>
-      <c r="P59" s="24">
+      <c r="P59" s="23">
         <v>4014</v>
       </c>
-      <c r="Q59" s="24">
+      <c r="Q59" s="23">
         <v>4043</v>
       </c>
-      <c r="R59" s="24">
+      <c r="R59" s="23">
         <v>4140</v>
       </c>
-      <c r="S59" s="24">
+      <c r="S59" s="23">
         <v>4037</v>
       </c>
     </row>
@@ -17778,23 +17770,23 @@
         <f t="shared" si="27"/>
         <v>8</v>
       </c>
-      <c r="N60" s="27">
+      <c r="N60" s="26">
         <f t="shared" si="18"/>
         <v>2794.6</v>
       </c>
-      <c r="O60" s="24">
+      <c r="O60" s="23">
         <v>2817</v>
       </c>
-      <c r="P60" s="24">
+      <c r="P60" s="23">
         <v>2807</v>
       </c>
-      <c r="Q60" s="24">
+      <c r="Q60" s="23">
         <v>2824</v>
       </c>
-      <c r="R60" s="24">
+      <c r="R60" s="23">
         <v>2823</v>
       </c>
-      <c r="S60" s="24">
+      <c r="S60" s="23">
         <v>2702</v>
       </c>
     </row>
@@ -17832,23 +17824,23 @@
         <f t="shared" si="27"/>
         <v>16</v>
       </c>
-      <c r="N61" s="27">
+      <c r="N61" s="26">
         <f t="shared" si="18"/>
         <v>1836.6</v>
       </c>
-      <c r="O61" s="24">
+      <c r="O61" s="23">
         <v>1890</v>
       </c>
-      <c r="P61" s="24">
+      <c r="P61" s="23">
         <v>1830</v>
       </c>
-      <c r="Q61" s="24">
+      <c r="Q61" s="23">
         <v>1816</v>
       </c>
-      <c r="R61" s="24">
+      <c r="R61" s="23">
         <v>1836</v>
       </c>
-      <c r="S61" s="24">
+      <c r="S61" s="23">
         <v>1811</v>
       </c>
     </row>
@@ -17886,23 +17878,23 @@
         <f t="shared" si="27"/>
         <v>32</v>
       </c>
-      <c r="N62" s="27">
+      <c r="N62" s="26">
         <f t="shared" si="18"/>
         <v>1439.4</v>
       </c>
-      <c r="O62" s="24">
+      <c r="O62" s="23">
         <v>1436</v>
       </c>
-      <c r="P62" s="24">
+      <c r="P62" s="23">
         <v>1411</v>
       </c>
-      <c r="Q62" s="24">
+      <c r="Q62" s="23">
         <v>1368</v>
       </c>
-      <c r="R62" s="24">
+      <c r="R62" s="23">
         <v>1474</v>
       </c>
-      <c r="S62" s="24">
+      <c r="S62" s="23">
         <v>1508</v>
       </c>
     </row>
@@ -17940,23 +17932,23 @@
         <f t="shared" si="27"/>
         <v>64</v>
       </c>
-      <c r="N63" s="27">
+      <c r="N63" s="26">
         <f t="shared" si="18"/>
         <v>1263.5999999999999</v>
       </c>
-      <c r="O63" s="24">
+      <c r="O63" s="23">
         <v>1259</v>
       </c>
-      <c r="P63" s="24">
+      <c r="P63" s="23">
         <v>1254</v>
       </c>
-      <c r="Q63" s="24">
+      <c r="Q63" s="23">
         <v>1227</v>
       </c>
-      <c r="R63" s="24">
+      <c r="R63" s="23">
         <v>1284</v>
       </c>
-      <c r="S63" s="24">
+      <c r="S63" s="23">
         <v>1294</v>
       </c>
     </row>
@@ -17994,23 +17986,23 @@
         <f t="shared" si="27"/>
         <v>128</v>
       </c>
-      <c r="N64" s="27">
+      <c r="N64" s="26">
         <f t="shared" si="18"/>
         <v>1218.5999999999999</v>
       </c>
-      <c r="O64" s="24">
+      <c r="O64" s="23">
         <v>1281</v>
       </c>
-      <c r="P64" s="24">
+      <c r="P64" s="23">
         <v>1234</v>
       </c>
-      <c r="Q64" s="24">
+      <c r="Q64" s="23">
         <v>1193</v>
       </c>
-      <c r="R64" s="24">
+      <c r="R64" s="23">
         <v>1210</v>
       </c>
-      <c r="S64" s="24">
+      <c r="S64" s="23">
         <v>1175</v>
       </c>
     </row>
@@ -18048,23 +18040,23 @@
         <f t="shared" si="27"/>
         <v>256</v>
       </c>
-      <c r="N65" s="27">
+      <c r="N65" s="26">
         <f t="shared" si="18"/>
         <v>1184.4000000000001</v>
       </c>
-      <c r="O65" s="24">
+      <c r="O65" s="23">
         <v>1204</v>
       </c>
-      <c r="P65" s="24">
+      <c r="P65" s="23">
         <v>1170</v>
       </c>
-      <c r="Q65" s="24">
+      <c r="Q65" s="23">
         <v>1184</v>
       </c>
-      <c r="R65" s="24">
+      <c r="R65" s="23">
         <v>1206</v>
       </c>
-      <c r="S65" s="24">
+      <c r="S65" s="23">
         <v>1158</v>
       </c>
     </row>
@@ -18102,23 +18094,23 @@
         <f t="shared" si="27"/>
         <v>512</v>
       </c>
-      <c r="N66" s="27">
+      <c r="N66" s="26">
         <f t="shared" si="18"/>
         <v>1286</v>
       </c>
-      <c r="O66" s="24">
+      <c r="O66" s="23">
         <v>1268</v>
       </c>
-      <c r="P66" s="24">
+      <c r="P66" s="23">
         <v>1282</v>
       </c>
-      <c r="Q66" s="24">
+      <c r="Q66" s="23">
         <v>1253</v>
       </c>
-      <c r="R66" s="24">
+      <c r="R66" s="23">
         <v>1312</v>
       </c>
-      <c r="S66" s="24">
+      <c r="S66" s="23">
         <v>1315</v>
       </c>
     </row>
@@ -18156,23 +18148,23 @@
         <f t="shared" si="27"/>
         <v>1024</v>
       </c>
-      <c r="N67" s="27">
+      <c r="N67" s="26">
         <f t="shared" si="18"/>
         <v>1581</v>
       </c>
-      <c r="O67" s="24">
+      <c r="O67" s="23">
         <v>1656</v>
       </c>
-      <c r="P67" s="24">
+      <c r="P67" s="23">
         <v>1539</v>
       </c>
-      <c r="Q67" s="24">
+      <c r="Q67" s="23">
         <v>1588</v>
       </c>
-      <c r="R67" s="24">
+      <c r="R67" s="23">
         <v>1539</v>
       </c>
-      <c r="S67" s="24">
+      <c r="S67" s="23">
         <v>1583</v>
       </c>
     </row>
@@ -18210,23 +18202,23 @@
         <f t="shared" si="27"/>
         <v>2048</v>
       </c>
-      <c r="N68" s="27">
+      <c r="N68" s="26">
         <f t="shared" si="18"/>
         <v>2646.6</v>
       </c>
-      <c r="O68" s="24">
+      <c r="O68" s="23">
         <v>2692</v>
       </c>
-      <c r="P68" s="24">
+      <c r="P68" s="23">
         <v>2590</v>
       </c>
-      <c r="Q68" s="24">
+      <c r="Q68" s="23">
         <v>2752</v>
       </c>
-      <c r="R68" s="24">
+      <c r="R68" s="23">
         <v>2583</v>
       </c>
-      <c r="S68" s="24">
+      <c r="S68" s="23">
         <v>2616</v>
       </c>
     </row>
@@ -18262,23 +18254,23 @@
       <c r="M69" s="6">
         <v>1</v>
       </c>
-      <c r="N69" s="27">
+      <c r="N69" s="26">
         <f t="shared" si="18"/>
         <v>6077</v>
       </c>
-      <c r="O69" s="24">
+      <c r="O69" s="23">
         <v>6110</v>
       </c>
-      <c r="P69" s="24">
+      <c r="P69" s="23">
         <v>6058</v>
       </c>
-      <c r="Q69" s="24">
+      <c r="Q69" s="23">
         <v>6054</v>
       </c>
-      <c r="R69" s="24">
+      <c r="R69" s="23">
         <v>6025</v>
       </c>
-      <c r="S69" s="24">
+      <c r="S69" s="23">
         <v>6138</v>
       </c>
     </row>
@@ -18316,23 +18308,23 @@
         <f t="shared" ref="M70:M80" si="29">M69*2</f>
         <v>2</v>
       </c>
-      <c r="N70" s="27">
+      <c r="N70" s="26">
         <f t="shared" si="18"/>
         <v>5554.8</v>
       </c>
-      <c r="O70" s="24">
+      <c r="O70" s="23">
         <v>5554</v>
       </c>
-      <c r="P70" s="24">
+      <c r="P70" s="23">
         <v>5577</v>
       </c>
-      <c r="Q70" s="24">
+      <c r="Q70" s="23">
         <v>5555</v>
       </c>
-      <c r="R70" s="24">
+      <c r="R70" s="23">
         <v>5506</v>
       </c>
-      <c r="S70" s="24">
+      <c r="S70" s="23">
         <v>5582</v>
       </c>
     </row>
@@ -18370,23 +18362,23 @@
         <f t="shared" si="29"/>
         <v>4</v>
       </c>
-      <c r="N71" s="27">
+      <c r="N71" s="26">
         <f t="shared" si="18"/>
         <v>4084.6</v>
       </c>
-      <c r="O71" s="24">
+      <c r="O71" s="23">
         <v>4146</v>
       </c>
-      <c r="P71" s="24">
+      <c r="P71" s="23">
         <v>4104</v>
       </c>
-      <c r="Q71" s="24">
+      <c r="Q71" s="23">
         <v>4018</v>
       </c>
-      <c r="R71" s="24">
+      <c r="R71" s="23">
         <v>4073</v>
       </c>
-      <c r="S71" s="24">
+      <c r="S71" s="23">
         <v>4082</v>
       </c>
     </row>
@@ -18424,23 +18416,23 @@
         <f t="shared" si="29"/>
         <v>8</v>
       </c>
-      <c r="N72" s="27">
+      <c r="N72" s="26">
         <f t="shared" si="18"/>
         <v>2803.8</v>
       </c>
-      <c r="O72" s="24">
+      <c r="O72" s="23">
         <v>2820</v>
       </c>
-      <c r="P72" s="24">
+      <c r="P72" s="23">
         <v>2797</v>
       </c>
-      <c r="Q72" s="24">
+      <c r="Q72" s="23">
         <v>2815</v>
       </c>
-      <c r="R72" s="24">
+      <c r="R72" s="23">
         <v>2758</v>
       </c>
-      <c r="S72" s="24">
+      <c r="S72" s="23">
         <v>2829</v>
       </c>
     </row>
@@ -18478,23 +18470,23 @@
         <f t="shared" si="29"/>
         <v>16</v>
       </c>
-      <c r="N73" s="27">
+      <c r="N73" s="26">
         <f t="shared" si="18"/>
         <v>1857.6</v>
       </c>
-      <c r="O73" s="24">
+      <c r="O73" s="23">
         <v>1880</v>
       </c>
-      <c r="P73" s="24">
+      <c r="P73" s="23">
         <v>1860</v>
       </c>
-      <c r="Q73" s="24">
+      <c r="Q73" s="23">
         <v>1848</v>
       </c>
-      <c r="R73" s="24">
+      <c r="R73" s="23">
         <v>1874</v>
       </c>
-      <c r="S73" s="24">
+      <c r="S73" s="23">
         <v>1826</v>
       </c>
     </row>
@@ -18532,23 +18524,23 @@
         <f t="shared" si="29"/>
         <v>32</v>
       </c>
-      <c r="N74" s="27">
+      <c r="N74" s="26">
         <f t="shared" si="18"/>
         <v>1423.2</v>
       </c>
-      <c r="O74" s="24">
+      <c r="O74" s="23">
         <v>1478</v>
       </c>
-      <c r="P74" s="24">
+      <c r="P74" s="23">
         <v>1407</v>
       </c>
-      <c r="Q74" s="24">
+      <c r="Q74" s="23">
         <v>1375</v>
       </c>
-      <c r="R74" s="24">
+      <c r="R74" s="23">
         <v>1445</v>
       </c>
-      <c r="S74" s="24">
+      <c r="S74" s="23">
         <v>1411</v>
       </c>
     </row>
@@ -18586,23 +18578,23 @@
         <f t="shared" si="29"/>
         <v>64</v>
       </c>
-      <c r="N75" s="27">
+      <c r="N75" s="26">
         <f t="shared" si="18"/>
         <v>1298.5999999999999</v>
       </c>
-      <c r="O75" s="24">
+      <c r="O75" s="23">
         <v>1332</v>
       </c>
-      <c r="P75" s="24">
+      <c r="P75" s="23">
         <v>1329</v>
       </c>
-      <c r="Q75" s="24">
+      <c r="Q75" s="23">
         <v>1302</v>
       </c>
-      <c r="R75" s="24">
+      <c r="R75" s="23">
         <v>1237</v>
       </c>
-      <c r="S75" s="24">
+      <c r="S75" s="23">
         <v>1293</v>
       </c>
     </row>
@@ -18640,23 +18632,23 @@
         <f t="shared" si="29"/>
         <v>128</v>
       </c>
-      <c r="N76" s="27">
+      <c r="N76" s="26">
         <f t="shared" si="18"/>
         <v>1252</v>
       </c>
-      <c r="O76" s="24">
+      <c r="O76" s="23">
         <v>1261</v>
       </c>
-      <c r="P76" s="24">
+      <c r="P76" s="23">
         <v>1235</v>
       </c>
-      <c r="Q76" s="24">
+      <c r="Q76" s="23">
         <v>1219</v>
       </c>
-      <c r="R76" s="24">
+      <c r="R76" s="23">
         <v>1310</v>
       </c>
-      <c r="S76" s="24">
+      <c r="S76" s="23">
         <v>1235</v>
       </c>
     </row>
@@ -18694,23 +18686,23 @@
         <f t="shared" si="29"/>
         <v>256</v>
       </c>
-      <c r="N77" s="27">
+      <c r="N77" s="26">
         <f t="shared" si="18"/>
         <v>1293.2</v>
       </c>
-      <c r="O77" s="24">
+      <c r="O77" s="23">
         <v>1247</v>
       </c>
-      <c r="P77" s="24">
+      <c r="P77" s="23">
         <v>1306</v>
       </c>
-      <c r="Q77" s="24">
+      <c r="Q77" s="23">
         <v>1313</v>
       </c>
-      <c r="R77" s="24">
+      <c r="R77" s="23">
         <v>1302</v>
       </c>
-      <c r="S77" s="24">
+      <c r="S77" s="23">
         <v>1298</v>
       </c>
     </row>
@@ -18748,23 +18740,23 @@
         <f t="shared" si="29"/>
         <v>512</v>
       </c>
-      <c r="N78" s="27">
+      <c r="N78" s="26">
         <f t="shared" si="18"/>
         <v>1362.8</v>
       </c>
-      <c r="O78" s="24">
+      <c r="O78" s="23">
         <v>1321</v>
       </c>
-      <c r="P78" s="24">
+      <c r="P78" s="23">
         <v>1348</v>
       </c>
-      <c r="Q78" s="24">
+      <c r="Q78" s="23">
         <v>1381</v>
       </c>
-      <c r="R78" s="24">
+      <c r="R78" s="23">
         <v>1370</v>
       </c>
-      <c r="S78" s="24">
+      <c r="S78" s="23">
         <v>1394</v>
       </c>
     </row>
@@ -18802,23 +18794,23 @@
         <f t="shared" si="29"/>
         <v>1024</v>
       </c>
-      <c r="N79" s="27">
+      <c r="N79" s="26">
         <f t="shared" si="18"/>
         <v>1610.6</v>
       </c>
-      <c r="O79" s="24">
+      <c r="O79" s="23">
         <v>1567</v>
       </c>
-      <c r="P79" s="24">
+      <c r="P79" s="23">
         <v>1570</v>
       </c>
-      <c r="Q79" s="24">
+      <c r="Q79" s="23">
         <v>1623</v>
       </c>
-      <c r="R79" s="24">
+      <c r="R79" s="23">
         <v>1628</v>
       </c>
-      <c r="S79" s="24">
+      <c r="S79" s="23">
         <v>1665</v>
       </c>
     </row>
@@ -18856,23 +18848,23 @@
         <f t="shared" si="29"/>
         <v>2048</v>
       </c>
-      <c r="N80" s="27">
+      <c r="N80" s="26">
         <f t="shared" si="18"/>
         <v>2547.6</v>
       </c>
-      <c r="O80" s="24">
+      <c r="O80" s="23">
         <v>2505</v>
       </c>
-      <c r="P80" s="24">
+      <c r="P80" s="23">
         <v>2591</v>
       </c>
-      <c r="Q80" s="24">
+      <c r="Q80" s="23">
         <v>2530</v>
       </c>
-      <c r="R80" s="24">
+      <c r="R80" s="23">
         <v>2546</v>
       </c>
-      <c r="S80" s="24">
+      <c r="S80" s="23">
         <v>2566</v>
       </c>
     </row>
@@ -18908,23 +18900,23 @@
       <c r="M81" s="6">
         <v>1</v>
       </c>
-      <c r="N81" s="27">
+      <c r="N81" s="26">
         <f t="shared" si="18"/>
         <v>6103.4</v>
       </c>
-      <c r="O81" s="24">
+      <c r="O81" s="23">
         <v>6254</v>
       </c>
-      <c r="P81" s="24">
+      <c r="P81" s="23">
         <v>6075</v>
       </c>
-      <c r="Q81" s="24">
+      <c r="Q81" s="23">
         <v>6147</v>
       </c>
-      <c r="R81" s="24">
+      <c r="R81" s="23">
         <v>5994</v>
       </c>
-      <c r="S81" s="24">
+      <c r="S81" s="23">
         <v>6047</v>
       </c>
     </row>
@@ -18962,23 +18954,23 @@
         <f t="shared" ref="M82:M92" si="31">M81*2</f>
         <v>2</v>
       </c>
-      <c r="N82" s="27">
+      <c r="N82" s="26">
         <f t="shared" si="18"/>
         <v>5535</v>
       </c>
-      <c r="O82" s="24">
+      <c r="O82" s="23">
         <v>5510</v>
       </c>
-      <c r="P82" s="24">
+      <c r="P82" s="23">
         <v>5743</v>
       </c>
-      <c r="Q82" s="24">
+      <c r="Q82" s="23">
         <v>5336</v>
       </c>
-      <c r="R82" s="24">
+      <c r="R82" s="23">
         <v>5566</v>
       </c>
-      <c r="S82" s="24">
+      <c r="S82" s="23">
         <v>5520</v>
       </c>
     </row>
@@ -19016,23 +19008,23 @@
         <f t="shared" si="31"/>
         <v>4</v>
       </c>
-      <c r="N83" s="27">
+      <c r="N83" s="26">
         <f t="shared" si="18"/>
         <v>4091.4</v>
       </c>
-      <c r="O83" s="24">
+      <c r="O83" s="23">
         <v>4173</v>
       </c>
-      <c r="P83" s="24">
+      <c r="P83" s="23">
         <v>4051</v>
       </c>
-      <c r="Q83" s="24">
+      <c r="Q83" s="23">
         <v>4074</v>
       </c>
-      <c r="R83" s="24">
+      <c r="R83" s="23">
         <v>4123</v>
       </c>
-      <c r="S83" s="24">
+      <c r="S83" s="23">
         <v>4036</v>
       </c>
     </row>
@@ -19070,23 +19062,23 @@
         <f t="shared" si="31"/>
         <v>8</v>
       </c>
-      <c r="N84" s="27">
+      <c r="N84" s="26">
         <f t="shared" si="18"/>
         <v>2829.2</v>
       </c>
-      <c r="O84" s="24">
+      <c r="O84" s="23">
         <v>2840</v>
       </c>
-      <c r="P84" s="24">
+      <c r="P84" s="23">
         <v>2809</v>
       </c>
-      <c r="Q84" s="24">
+      <c r="Q84" s="23">
         <v>2825</v>
       </c>
-      <c r="R84" s="24">
+      <c r="R84" s="23">
         <v>2832</v>
       </c>
-      <c r="S84" s="24">
+      <c r="S84" s="23">
         <v>2840</v>
       </c>
     </row>
@@ -19124,23 +19116,23 @@
         <f t="shared" si="31"/>
         <v>16</v>
       </c>
-      <c r="N85" s="27">
+      <c r="N85" s="26">
         <f t="shared" ref="N85:N116" si="32">AVERAGE(O85:S85)</f>
         <v>1908.2</v>
       </c>
-      <c r="O85" s="24">
+      <c r="O85" s="23">
         <v>1885</v>
       </c>
-      <c r="P85" s="24">
+      <c r="P85" s="23">
         <v>1865</v>
       </c>
-      <c r="Q85" s="24">
+      <c r="Q85" s="23">
         <v>1956</v>
       </c>
-      <c r="R85" s="24">
+      <c r="R85" s="23">
         <v>1930</v>
       </c>
-      <c r="S85" s="24">
+      <c r="S85" s="23">
         <v>1905</v>
       </c>
     </row>
@@ -19178,23 +19170,23 @@
         <f t="shared" si="31"/>
         <v>32</v>
       </c>
-      <c r="N86" s="27">
+      <c r="N86" s="26">
         <f t="shared" si="32"/>
         <v>1609</v>
       </c>
-      <c r="O86" s="24">
+      <c r="O86" s="23">
         <v>1567</v>
       </c>
-      <c r="P86" s="24">
+      <c r="P86" s="23">
         <v>1671</v>
       </c>
-      <c r="Q86" s="24">
+      <c r="Q86" s="23">
         <v>1600</v>
       </c>
-      <c r="R86" s="24">
+      <c r="R86" s="23">
         <v>1581</v>
       </c>
-      <c r="S86" s="24">
+      <c r="S86" s="23">
         <v>1626</v>
       </c>
     </row>
@@ -19232,23 +19224,23 @@
         <f t="shared" si="31"/>
         <v>64</v>
       </c>
-      <c r="N87" s="27">
+      <c r="N87" s="26">
         <f t="shared" si="32"/>
         <v>1470.6</v>
       </c>
-      <c r="O87" s="24">
+      <c r="O87" s="23">
         <v>1480</v>
       </c>
-      <c r="P87" s="24">
+      <c r="P87" s="23">
         <v>1461</v>
       </c>
-      <c r="Q87" s="24">
+      <c r="Q87" s="23">
         <v>1473</v>
       </c>
-      <c r="R87" s="24">
+      <c r="R87" s="23">
         <v>1480</v>
       </c>
-      <c r="S87" s="24">
+      <c r="S87" s="23">
         <v>1459</v>
       </c>
     </row>
@@ -19286,23 +19278,23 @@
         <f t="shared" si="31"/>
         <v>128</v>
       </c>
-      <c r="N88" s="27">
+      <c r="N88" s="26">
         <f t="shared" si="32"/>
         <v>1410.8</v>
       </c>
-      <c r="O88" s="24">
+      <c r="O88" s="23">
         <v>1410</v>
       </c>
-      <c r="P88" s="24">
+      <c r="P88" s="23">
         <v>1359</v>
       </c>
-      <c r="Q88" s="24">
+      <c r="Q88" s="23">
         <v>1410</v>
       </c>
-      <c r="R88" s="24">
+      <c r="R88" s="23">
         <v>1439</v>
       </c>
-      <c r="S88" s="24">
+      <c r="S88" s="23">
         <v>1436</v>
       </c>
     </row>
@@ -19340,23 +19332,23 @@
         <f t="shared" si="31"/>
         <v>256</v>
       </c>
-      <c r="N89" s="27">
+      <c r="N89" s="26">
         <f t="shared" si="32"/>
         <v>1437.4</v>
       </c>
-      <c r="O89" s="24">
+      <c r="O89" s="23">
         <v>1430</v>
       </c>
-      <c r="P89" s="24">
+      <c r="P89" s="23">
         <v>1423</v>
       </c>
-      <c r="Q89" s="24">
+      <c r="Q89" s="23">
         <v>1450</v>
       </c>
-      <c r="R89" s="24">
+      <c r="R89" s="23">
         <v>1466</v>
       </c>
-      <c r="S89" s="24">
+      <c r="S89" s="23">
         <v>1418</v>
       </c>
     </row>
@@ -19394,23 +19386,23 @@
         <f t="shared" si="31"/>
         <v>512</v>
       </c>
-      <c r="N90" s="27">
+      <c r="N90" s="26">
         <f t="shared" si="32"/>
         <v>1495</v>
       </c>
-      <c r="O90" s="24">
+      <c r="O90" s="23">
         <v>1519</v>
       </c>
-      <c r="P90" s="24">
+      <c r="P90" s="23">
         <v>1458</v>
       </c>
-      <c r="Q90" s="24">
+      <c r="Q90" s="23">
         <v>1527</v>
       </c>
-      <c r="R90" s="24">
+      <c r="R90" s="23">
         <v>1487</v>
       </c>
-      <c r="S90" s="24">
+      <c r="S90" s="23">
         <v>1484</v>
       </c>
     </row>
@@ -19448,23 +19440,23 @@
         <f t="shared" si="31"/>
         <v>1024</v>
       </c>
-      <c r="N91" s="27">
+      <c r="N91" s="26">
         <f t="shared" si="32"/>
         <v>1766.4</v>
       </c>
-      <c r="O91" s="24">
+      <c r="O91" s="23">
         <v>1754</v>
       </c>
-      <c r="P91" s="24">
+      <c r="P91" s="23">
         <v>1827</v>
       </c>
-      <c r="Q91" s="24">
+      <c r="Q91" s="23">
         <v>1737</v>
       </c>
-      <c r="R91" s="24">
+      <c r="R91" s="23">
         <v>1761</v>
       </c>
-      <c r="S91" s="24">
+      <c r="S91" s="23">
         <v>1753</v>
       </c>
     </row>
@@ -19502,23 +19494,23 @@
         <f t="shared" si="31"/>
         <v>2048</v>
       </c>
-      <c r="N92" s="27">
+      <c r="N92" s="26">
         <f t="shared" si="32"/>
         <v>2700.2</v>
       </c>
-      <c r="O92" s="24">
+      <c r="O92" s="23">
         <v>2730</v>
       </c>
-      <c r="P92" s="24">
+      <c r="P92" s="23">
         <v>2712</v>
       </c>
-      <c r="Q92" s="24">
+      <c r="Q92" s="23">
         <v>2716</v>
       </c>
-      <c r="R92" s="24">
+      <c r="R92" s="23">
         <v>2598</v>
       </c>
-      <c r="S92" s="24">
+      <c r="S92" s="23">
         <v>2745</v>
       </c>
     </row>
@@ -19554,23 +19546,23 @@
       <c r="M93" s="6">
         <v>1</v>
       </c>
-      <c r="N93" s="27">
+      <c r="N93" s="26">
         <f t="shared" si="32"/>
         <v>6052.8</v>
       </c>
-      <c r="O93" s="24">
+      <c r="O93" s="23">
         <v>5906</v>
       </c>
-      <c r="P93" s="24">
+      <c r="P93" s="23">
         <v>6026</v>
       </c>
-      <c r="Q93" s="24">
+      <c r="Q93" s="23">
         <v>6141</v>
       </c>
-      <c r="R93" s="24">
+      <c r="R93" s="23">
         <v>6116</v>
       </c>
-      <c r="S93" s="24">
+      <c r="S93" s="23">
         <v>6075</v>
       </c>
     </row>
@@ -19608,23 +19600,23 @@
         <f t="shared" ref="M94:M104" si="36">M93*2</f>
         <v>2</v>
       </c>
-      <c r="N94" s="27">
+      <c r="N94" s="26">
         <f t="shared" si="32"/>
         <v>5351.4</v>
       </c>
-      <c r="O94" s="24">
+      <c r="O94" s="23">
         <v>5351</v>
       </c>
-      <c r="P94" s="24">
+      <c r="P94" s="23">
         <v>5236</v>
       </c>
-      <c r="Q94" s="24">
+      <c r="Q94" s="23">
         <v>5214</v>
       </c>
-      <c r="R94" s="24">
+      <c r="R94" s="23">
         <v>5482</v>
       </c>
-      <c r="S94" s="24">
+      <c r="S94" s="23">
         <v>5474</v>
       </c>
     </row>
@@ -19662,23 +19654,23 @@
         <f t="shared" si="36"/>
         <v>4</v>
       </c>
-      <c r="N95" s="27">
+      <c r="N95" s="26">
         <f t="shared" si="32"/>
         <v>4131.6000000000004</v>
       </c>
-      <c r="O95" s="24">
+      <c r="O95" s="23">
         <v>4105</v>
       </c>
-      <c r="P95" s="24">
+      <c r="P95" s="23">
         <v>3994</v>
       </c>
-      <c r="Q95" s="24">
+      <c r="Q95" s="23">
         <v>4342</v>
       </c>
-      <c r="R95" s="24">
+      <c r="R95" s="23">
         <v>4075</v>
       </c>
-      <c r="S95" s="24">
+      <c r="S95" s="23">
         <v>4142</v>
       </c>
     </row>
@@ -19716,23 +19708,23 @@
         <f t="shared" si="36"/>
         <v>8</v>
       </c>
-      <c r="N96" s="27">
+      <c r="N96" s="26">
         <f t="shared" si="32"/>
         <v>2818.4</v>
       </c>
-      <c r="O96" s="24">
+      <c r="O96" s="23">
         <v>2828</v>
       </c>
-      <c r="P96" s="24">
+      <c r="P96" s="23">
         <v>2810</v>
       </c>
-      <c r="Q96" s="24">
+      <c r="Q96" s="23">
         <v>2868</v>
       </c>
-      <c r="R96" s="24">
+      <c r="R96" s="23">
         <v>2828</v>
       </c>
-      <c r="S96" s="24">
+      <c r="S96" s="23">
         <v>2758</v>
       </c>
     </row>
@@ -19770,23 +19762,23 @@
         <f t="shared" si="36"/>
         <v>16</v>
       </c>
-      <c r="N97" s="27">
+      <c r="N97" s="26">
         <f t="shared" si="32"/>
         <v>1955</v>
       </c>
-      <c r="O97" s="24">
+      <c r="O97" s="23">
         <v>1995</v>
       </c>
-      <c r="P97" s="24">
+      <c r="P97" s="23">
         <v>1997</v>
       </c>
-      <c r="Q97" s="24">
+      <c r="Q97" s="23">
         <v>1976</v>
       </c>
-      <c r="R97" s="24">
+      <c r="R97" s="23">
         <v>1916</v>
       </c>
-      <c r="S97" s="24">
+      <c r="S97" s="23">
         <v>1891</v>
       </c>
     </row>
@@ -19824,23 +19816,23 @@
         <f t="shared" si="36"/>
         <v>32</v>
       </c>
-      <c r="N98" s="27">
+      <c r="N98" s="26">
         <f t="shared" si="32"/>
         <v>1762.4</v>
       </c>
-      <c r="O98" s="24">
+      <c r="O98" s="23">
         <v>1758</v>
       </c>
-      <c r="P98" s="24">
+      <c r="P98" s="23">
         <v>1838</v>
       </c>
-      <c r="Q98" s="24">
+      <c r="Q98" s="23">
         <v>1669</v>
       </c>
-      <c r="R98" s="24">
+      <c r="R98" s="23">
         <v>1756</v>
       </c>
-      <c r="S98" s="24">
+      <c r="S98" s="23">
         <v>1791</v>
       </c>
     </row>
@@ -19878,23 +19870,23 @@
         <f t="shared" si="36"/>
         <v>64</v>
       </c>
-      <c r="N99" s="27">
+      <c r="N99" s="26">
         <f t="shared" si="32"/>
         <v>1717.8</v>
       </c>
-      <c r="O99" s="24">
+      <c r="O99" s="23">
         <v>1690</v>
       </c>
-      <c r="P99" s="24">
+      <c r="P99" s="23">
         <v>1670</v>
       </c>
-      <c r="Q99" s="24">
+      <c r="Q99" s="23">
         <v>1670</v>
       </c>
-      <c r="R99" s="24">
+      <c r="R99" s="23">
         <v>1820</v>
       </c>
-      <c r="S99" s="24">
+      <c r="S99" s="23">
         <v>1739</v>
       </c>
     </row>
@@ -19932,23 +19924,23 @@
         <f t="shared" si="36"/>
         <v>128</v>
       </c>
-      <c r="N100" s="27">
+      <c r="N100" s="26">
         <f t="shared" si="32"/>
         <v>1716</v>
       </c>
-      <c r="O100" s="24">
+      <c r="O100" s="23">
         <v>1751</v>
       </c>
-      <c r="P100" s="24">
+      <c r="P100" s="23">
         <v>1743</v>
       </c>
-      <c r="Q100" s="24">
+      <c r="Q100" s="23">
         <v>1695</v>
       </c>
-      <c r="R100" s="24">
+      <c r="R100" s="23">
         <v>1725</v>
       </c>
-      <c r="S100" s="24">
+      <c r="S100" s="23">
         <v>1666</v>
       </c>
     </row>
@@ -19986,23 +19978,23 @@
         <f t="shared" si="36"/>
         <v>256</v>
       </c>
-      <c r="N101" s="27">
+      <c r="N101" s="26">
         <f t="shared" si="32"/>
         <v>1697.2</v>
       </c>
-      <c r="O101" s="24">
+      <c r="O101" s="23">
         <v>1734</v>
       </c>
-      <c r="P101" s="24">
+      <c r="P101" s="23">
         <v>1660</v>
       </c>
-      <c r="Q101" s="24">
+      <c r="Q101" s="23">
         <v>1680</v>
       </c>
-      <c r="R101" s="24">
+      <c r="R101" s="23">
         <v>1700</v>
       </c>
-      <c r="S101" s="24">
+      <c r="S101" s="23">
         <v>1712</v>
       </c>
     </row>
@@ -20040,23 +20032,23 @@
         <f t="shared" si="36"/>
         <v>512</v>
       </c>
-      <c r="N102" s="27">
+      <c r="N102" s="26">
         <f t="shared" si="32"/>
         <v>1756.8</v>
       </c>
-      <c r="O102" s="24">
+      <c r="O102" s="23">
         <v>1770</v>
       </c>
-      <c r="P102" s="24">
+      <c r="P102" s="23">
         <v>1714</v>
       </c>
-      <c r="Q102" s="24">
+      <c r="Q102" s="23">
         <v>1794</v>
       </c>
-      <c r="R102" s="24">
+      <c r="R102" s="23">
         <v>1770</v>
       </c>
-      <c r="S102" s="24">
+      <c r="S102" s="23">
         <v>1736</v>
       </c>
     </row>
@@ -20094,23 +20086,23 @@
         <f t="shared" si="36"/>
         <v>1024</v>
       </c>
-      <c r="N103" s="27">
+      <c r="N103" s="26">
         <f t="shared" si="32"/>
         <v>2191.1999999999998</v>
       </c>
-      <c r="O103" s="24">
+      <c r="O103" s="23">
         <v>2010</v>
       </c>
-      <c r="P103" s="24">
+      <c r="P103" s="23">
         <v>1979</v>
       </c>
-      <c r="Q103" s="24">
+      <c r="Q103" s="23">
         <v>2025</v>
       </c>
-      <c r="R103" s="24">
+      <c r="R103" s="23">
         <v>2959</v>
       </c>
-      <c r="S103" s="24">
+      <c r="S103" s="23">
         <v>1983</v>
       </c>
     </row>
@@ -20148,23 +20140,23 @@
         <f t="shared" si="36"/>
         <v>2048</v>
       </c>
-      <c r="N104" s="27">
+      <c r="N104" s="26">
         <f t="shared" si="32"/>
         <v>2838.2</v>
       </c>
-      <c r="O104" s="24">
+      <c r="O104" s="23">
         <v>2921</v>
       </c>
-      <c r="P104" s="24">
+      <c r="P104" s="23">
         <v>2754</v>
       </c>
-      <c r="Q104" s="24">
+      <c r="Q104" s="23">
         <v>2903</v>
       </c>
-      <c r="R104" s="24">
+      <c r="R104" s="23">
         <v>2892</v>
       </c>
-      <c r="S104" s="24">
+      <c r="S104" s="23">
         <v>2721</v>
       </c>
     </row>
@@ -20200,23 +20192,23 @@
       <c r="M105" s="6">
         <v>1</v>
       </c>
-      <c r="N105" s="27">
+      <c r="N105" s="26">
         <f t="shared" si="32"/>
         <v>6067</v>
       </c>
-      <c r="O105" s="24">
+      <c r="O105" s="23">
         <v>6104</v>
       </c>
-      <c r="P105" s="24">
+      <c r="P105" s="23">
         <v>6036</v>
       </c>
-      <c r="Q105" s="24">
+      <c r="Q105" s="23">
         <v>6105</v>
       </c>
-      <c r="R105" s="24">
+      <c r="R105" s="23">
         <v>6018</v>
       </c>
-      <c r="S105" s="24">
+      <c r="S105" s="23">
         <v>6072</v>
       </c>
     </row>
@@ -20254,23 +20246,23 @@
         <f t="shared" ref="M106:M116" si="39">M105*2</f>
         <v>2</v>
       </c>
-      <c r="N106" s="27">
+      <c r="N106" s="26">
         <f t="shared" si="32"/>
         <v>5434</v>
       </c>
-      <c r="O106" s="24">
+      <c r="O106" s="23">
         <v>5321</v>
       </c>
-      <c r="P106" s="24">
+      <c r="P106" s="23">
         <v>5538</v>
       </c>
-      <c r="Q106" s="24">
+      <c r="Q106" s="23">
         <v>5547</v>
       </c>
-      <c r="R106" s="24">
+      <c r="R106" s="23">
         <v>5446</v>
       </c>
-      <c r="S106" s="24">
+      <c r="S106" s="23">
         <v>5318</v>
       </c>
     </row>
@@ -20308,23 +20300,23 @@
         <f t="shared" si="39"/>
         <v>4</v>
       </c>
-      <c r="N107" s="27">
+      <c r="N107" s="26">
         <f t="shared" si="32"/>
         <v>4103.6000000000004</v>
       </c>
-      <c r="O107" s="24">
+      <c r="O107" s="23">
         <v>4175</v>
       </c>
-      <c r="P107" s="24">
+      <c r="P107" s="23">
         <v>3962</v>
       </c>
-      <c r="Q107" s="24">
+      <c r="Q107" s="23">
         <v>4112</v>
       </c>
-      <c r="R107" s="24">
+      <c r="R107" s="23">
         <v>4028</v>
       </c>
-      <c r="S107" s="24">
+      <c r="S107" s="23">
         <v>4241</v>
       </c>
     </row>
@@ -20362,23 +20354,23 @@
         <f t="shared" si="39"/>
         <v>8</v>
       </c>
-      <c r="N108" s="27">
+      <c r="N108" s="26">
         <f t="shared" si="32"/>
         <v>2840</v>
       </c>
-      <c r="O108" s="24">
+      <c r="O108" s="23">
         <v>2823</v>
       </c>
-      <c r="P108" s="24">
+      <c r="P108" s="23">
         <v>2893</v>
       </c>
-      <c r="Q108" s="24">
+      <c r="Q108" s="23">
         <v>2787</v>
       </c>
-      <c r="R108" s="24">
+      <c r="R108" s="23">
         <v>2849</v>
       </c>
-      <c r="S108" s="24">
+      <c r="S108" s="23">
         <v>2848</v>
       </c>
     </row>
@@ -20416,23 +20408,23 @@
         <f t="shared" si="39"/>
         <v>16</v>
       </c>
-      <c r="N109" s="27">
+      <c r="N109" s="26">
         <f t="shared" si="32"/>
         <v>2220</v>
       </c>
-      <c r="O109" s="24">
+      <c r="O109" s="23">
         <v>2200</v>
       </c>
-      <c r="P109" s="24">
+      <c r="P109" s="23">
         <v>2155</v>
       </c>
-      <c r="Q109" s="24">
+      <c r="Q109" s="23">
         <v>2229</v>
       </c>
-      <c r="R109" s="24">
+      <c r="R109" s="23">
         <v>2360</v>
       </c>
-      <c r="S109" s="24">
+      <c r="S109" s="23">
         <v>2156</v>
       </c>
     </row>
@@ -20470,23 +20462,23 @@
         <f t="shared" si="39"/>
         <v>32</v>
       </c>
-      <c r="N110" s="27">
+      <c r="N110" s="26">
         <f t="shared" si="32"/>
         <v>2327.8000000000002</v>
       </c>
-      <c r="O110" s="24">
+      <c r="O110" s="23">
         <v>2461</v>
       </c>
-      <c r="P110" s="24">
+      <c r="P110" s="23">
         <v>2409</v>
       </c>
-      <c r="Q110" s="24">
+      <c r="Q110" s="23">
         <v>2158</v>
       </c>
-      <c r="R110" s="24">
+      <c r="R110" s="23">
         <v>2326</v>
       </c>
-      <c r="S110" s="24">
+      <c r="S110" s="23">
         <v>2285</v>
       </c>
     </row>
@@ -20524,23 +20516,23 @@
         <f t="shared" si="39"/>
         <v>64</v>
       </c>
-      <c r="N111" s="27">
+      <c r="N111" s="26">
         <f t="shared" si="32"/>
         <v>2338</v>
       </c>
-      <c r="O111" s="24">
+      <c r="O111" s="23">
         <v>2368</v>
       </c>
-      <c r="P111" s="24">
+      <c r="P111" s="23">
         <v>2400</v>
       </c>
-      <c r="Q111" s="24">
+      <c r="Q111" s="23">
         <v>2270</v>
       </c>
-      <c r="R111" s="24">
+      <c r="R111" s="23">
         <v>2259</v>
       </c>
-      <c r="S111" s="24">
+      <c r="S111" s="23">
         <v>2393</v>
       </c>
     </row>
@@ -20578,23 +20570,23 @@
         <f t="shared" si="39"/>
         <v>128</v>
       </c>
-      <c r="N112" s="27">
+      <c r="N112" s="26">
         <f t="shared" si="32"/>
         <v>2265.1999999999998</v>
       </c>
-      <c r="O112" s="24">
+      <c r="O112" s="23">
         <v>2270</v>
       </c>
-      <c r="P112" s="24">
+      <c r="P112" s="23">
         <v>2252</v>
       </c>
-      <c r="Q112" s="24">
+      <c r="Q112" s="23">
         <v>2272</v>
       </c>
-      <c r="R112" s="24">
+      <c r="R112" s="23">
         <v>2278</v>
       </c>
-      <c r="S112" s="24">
+      <c r="S112" s="23">
         <v>2254</v>
       </c>
     </row>
@@ -20632,23 +20624,23 @@
         <f t="shared" si="39"/>
         <v>256</v>
       </c>
-      <c r="N113" s="27">
+      <c r="N113" s="26">
         <f t="shared" si="32"/>
         <v>2268.4</v>
       </c>
-      <c r="O113" s="24">
+      <c r="O113" s="23">
         <v>2375</v>
       </c>
-      <c r="P113" s="24">
+      <c r="P113" s="23">
         <v>2279</v>
       </c>
-      <c r="Q113" s="24">
+      <c r="Q113" s="23">
         <v>2228</v>
       </c>
-      <c r="R113" s="24">
+      <c r="R113" s="23">
         <v>2242</v>
       </c>
-      <c r="S113" s="24">
+      <c r="S113" s="23">
         <v>2218</v>
       </c>
     </row>
@@ -20686,23 +20678,23 @@
         <f t="shared" si="39"/>
         <v>512</v>
       </c>
-      <c r="N114" s="27">
+      <c r="N114" s="26">
         <f t="shared" si="32"/>
         <v>2303</v>
       </c>
-      <c r="O114" s="24">
+      <c r="O114" s="23">
         <v>2303</v>
       </c>
-      <c r="P114" s="24">
+      <c r="P114" s="23">
         <v>2289</v>
       </c>
-      <c r="Q114" s="24">
+      <c r="Q114" s="23">
         <v>2331</v>
       </c>
-      <c r="R114" s="24">
+      <c r="R114" s="23">
         <v>2332</v>
       </c>
-      <c r="S114" s="24">
+      <c r="S114" s="23">
         <v>2260</v>
       </c>
     </row>
@@ -20740,23 +20732,23 @@
         <f t="shared" si="39"/>
         <v>1024</v>
       </c>
-      <c r="N115" s="27">
+      <c r="N115" s="26">
         <f t="shared" si="32"/>
         <v>2521.6</v>
       </c>
-      <c r="O115" s="24">
+      <c r="O115" s="23">
         <v>2541</v>
       </c>
-      <c r="P115" s="24">
+      <c r="P115" s="23">
         <v>2505</v>
       </c>
-      <c r="Q115" s="24">
+      <c r="Q115" s="23">
         <v>2505</v>
       </c>
-      <c r="R115" s="24">
+      <c r="R115" s="23">
         <v>2541</v>
       </c>
-      <c r="S115" s="24">
+      <c r="S115" s="23">
         <v>2516</v>
       </c>
     </row>
@@ -20795,23 +20787,23 @@
         <f t="shared" si="39"/>
         <v>2048</v>
       </c>
-      <c r="N116" s="27">
+      <c r="N116" s="26">
         <f t="shared" si="32"/>
         <v>3360.2</v>
       </c>
-      <c r="O116" s="24">
+      <c r="O116" s="23">
         <v>3359</v>
       </c>
-      <c r="P116" s="24">
+      <c r="P116" s="23">
         <v>3381</v>
       </c>
-      <c r="Q116" s="24">
+      <c r="Q116" s="23">
         <v>3410</v>
       </c>
-      <c r="R116" s="24">
+      <c r="R116" s="23">
         <v>3305</v>
       </c>
-      <c r="S116" s="24">
+      <c r="S116" s="23">
         <v>3346</v>
       </c>
     </row>

</xml_diff>